<commit_message>
No longer adds optional tables in (#31). Implemented by adding then removing.
</commit_message>
<xml_diff>
--- a/data-raw/flexfile-tables.xlsx
+++ b/data-raw/flexfile-tables.xlsx
@@ -11,7 +11,7 @@
     <sheet name="fields" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">fields!$A$1:$H$172</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">fields!$A$1:$I$172</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="307">
   <si>
     <t>table</t>
   </si>
@@ -941,6 +941,9 @@
   </si>
   <si>
     <t>enum</t>
+  </si>
+  <si>
+    <t>optional</t>
   </si>
 </sst>
 </file>
@@ -2436,10 +2439,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H172"/>
+  <dimension ref="A1:I172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2455,7 +2458,7 @@
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2480,8 +2483,11 @@
       <c r="H1" s="3" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>291</v>
       </c>
@@ -2497,8 +2503,11 @@
       <c r="F2" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>291</v>
       </c>
@@ -2514,8 +2523,11 @@
       <c r="F3" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>293</v>
       </c>
@@ -2537,8 +2549,11 @@
       <c r="H4" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>293</v>
       </c>
@@ -2560,8 +2575,11 @@
       <c r="H5" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>293</v>
       </c>
@@ -2583,8 +2601,11 @@
       <c r="H6" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>293</v>
       </c>
@@ -2606,8 +2627,11 @@
       <c r="H7" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>293</v>
       </c>
@@ -2629,8 +2653,11 @@
       <c r="H8" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>293</v>
       </c>
@@ -2652,8 +2679,11 @@
       <c r="H9" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>293</v>
       </c>
@@ -2675,8 +2705,11 @@
       <c r="H10" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>293</v>
       </c>
@@ -2698,8 +2731,11 @@
       <c r="H11" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>293</v>
       </c>
@@ -2721,8 +2757,11 @@
       <c r="H12" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>293</v>
       </c>
@@ -2744,8 +2783,11 @@
       <c r="H13" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>293</v>
       </c>
@@ -2767,8 +2809,11 @@
       <c r="H14" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>293</v>
       </c>
@@ -2790,8 +2835,11 @@
       <c r="H15" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>293</v>
       </c>
@@ -2813,8 +2861,11 @@
       <c r="H16" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I16" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>293</v>
       </c>
@@ -2830,8 +2881,11 @@
       <c r="F17" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I17" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>293</v>
       </c>
@@ -2847,8 +2901,11 @@
       <c r="F18" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I18" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>293</v>
       </c>
@@ -2864,8 +2921,11 @@
       <c r="F19" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I19" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>293</v>
       </c>
@@ -2881,8 +2941,11 @@
       <c r="F20" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I20" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>293</v>
       </c>
@@ -2898,8 +2961,11 @@
       <c r="F21" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I21" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>293</v>
       </c>
@@ -2915,8 +2981,11 @@
       <c r="F22" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I22" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>293</v>
       </c>
@@ -2932,8 +3001,11 @@
       <c r="F23" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I23" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>293</v>
       </c>
@@ -2949,8 +3021,11 @@
       <c r="F24" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I24" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>293</v>
       </c>
@@ -2966,8 +3041,11 @@
       <c r="F25" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I25" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>293</v>
       </c>
@@ -2983,8 +3061,11 @@
       <c r="F26" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I26" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>293</v>
       </c>
@@ -3000,8 +3081,11 @@
       <c r="F27" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I27" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>293</v>
       </c>
@@ -3017,8 +3101,11 @@
       <c r="F28" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I28" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>293</v>
       </c>
@@ -3034,8 +3121,11 @@
       <c r="F29" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I29" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>293</v>
       </c>
@@ -3051,8 +3141,11 @@
       <c r="F30" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I30" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>293</v>
       </c>
@@ -3068,8 +3161,11 @@
       <c r="F31" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I31" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>293</v>
       </c>
@@ -3085,8 +3181,11 @@
       <c r="F32" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>293</v>
       </c>
@@ -3102,8 +3201,11 @@
       <c r="F33" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>293</v>
       </c>
@@ -3119,8 +3221,11 @@
       <c r="F34" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>293</v>
       </c>
@@ -3136,8 +3241,11 @@
       <c r="F35" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>293</v>
       </c>
@@ -3153,8 +3261,11 @@
       <c r="F36" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>293</v>
       </c>
@@ -3170,8 +3281,11 @@
       <c r="F37" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>293</v>
       </c>
@@ -3187,8 +3301,11 @@
       <c r="F38" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>293</v>
       </c>
@@ -3204,8 +3321,11 @@
       <c r="F39" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>293</v>
       </c>
@@ -3221,8 +3341,11 @@
       <c r="F40" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>293</v>
       </c>
@@ -3238,8 +3361,11 @@
       <c r="F41" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>293</v>
       </c>
@@ -3255,8 +3381,11 @@
       <c r="F42" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>293</v>
       </c>
@@ -3272,8 +3401,11 @@
       <c r="F43" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>281</v>
       </c>
@@ -3295,8 +3427,11 @@
       <c r="H44" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>281</v>
       </c>
@@ -3318,8 +3453,11 @@
       <c r="H45" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>281</v>
       </c>
@@ -3341,8 +3479,11 @@
       <c r="H46" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>281</v>
       </c>
@@ -3364,8 +3505,11 @@
       <c r="H47" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>281</v>
       </c>
@@ -3387,8 +3531,11 @@
       <c r="H48" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>281</v>
       </c>
@@ -3404,8 +3551,11 @@
       <c r="F49" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>280</v>
       </c>
@@ -3421,8 +3571,11 @@
       <c r="F50" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>280</v>
       </c>
@@ -3444,8 +3597,11 @@
       <c r="H51" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>280</v>
       </c>
@@ -3461,8 +3617,11 @@
       <c r="F52" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>280</v>
       </c>
@@ -3478,8 +3637,11 @@
       <c r="F53" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>294</v>
       </c>
@@ -3495,8 +3657,11 @@
       <c r="F54" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>294</v>
       </c>
@@ -3512,8 +3677,11 @@
       <c r="F55" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>294</v>
       </c>
@@ -3535,8 +3703,11 @@
       <c r="H56" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>289</v>
       </c>
@@ -3558,8 +3729,11 @@
       <c r="H57" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>289</v>
       </c>
@@ -3575,8 +3749,11 @@
       <c r="F58" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>289</v>
       </c>
@@ -3595,8 +3772,11 @@
       <c r="F59" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>295</v>
       </c>
@@ -3612,8 +3792,11 @@
       <c r="F60" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>295</v>
       </c>
@@ -3629,8 +3812,11 @@
       <c r="F61" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>301</v>
       </c>
@@ -3652,8 +3838,11 @@
       <c r="H62" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>301</v>
       </c>
@@ -3675,8 +3864,11 @@
       <c r="H63" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>301</v>
       </c>
@@ -3698,8 +3890,11 @@
       <c r="H64" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>301</v>
       </c>
@@ -3721,8 +3916,11 @@
       <c r="H65" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>301</v>
       </c>
@@ -3744,8 +3942,11 @@
       <c r="H66" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>301</v>
       </c>
@@ -3761,8 +3962,11 @@
       <c r="F67" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>301</v>
       </c>
@@ -3778,8 +3982,11 @@
       <c r="F68" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>296</v>
       </c>
@@ -3795,8 +4002,11 @@
       <c r="F69" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>296</v>
       </c>
@@ -3812,8 +4022,11 @@
       <c r="F70" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>297</v>
       </c>
@@ -3829,8 +4042,11 @@
       <c r="F71" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>297</v>
       </c>
@@ -3846,8 +4062,11 @@
       <c r="F72" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>303</v>
       </c>
@@ -3863,8 +4082,11 @@
       <c r="F73" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>303</v>
       </c>
@@ -3880,8 +4102,11 @@
       <c r="F74" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>303</v>
       </c>
@@ -3903,8 +4128,11 @@
       <c r="H75" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>303</v>
       </c>
@@ -3920,8 +4148,11 @@
       <c r="F76" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>303</v>
       </c>
@@ -3943,8 +4174,11 @@
       <c r="H77" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>303</v>
       </c>
@@ -3960,8 +4194,11 @@
       <c r="F78" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>303</v>
       </c>
@@ -3977,8 +4214,11 @@
       <c r="F79" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>303</v>
       </c>
@@ -3994,8 +4234,11 @@
       <c r="F80" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I80" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>303</v>
       </c>
@@ -4011,8 +4254,11 @@
       <c r="F81" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I81" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>303</v>
       </c>
@@ -4034,8 +4280,11 @@
       <c r="H82" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I82" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>275</v>
       </c>
@@ -4051,8 +4300,11 @@
       <c r="F83" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I83" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>275</v>
       </c>
@@ -4068,8 +4320,11 @@
       <c r="F84" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I84" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>275</v>
       </c>
@@ -4085,8 +4340,11 @@
       <c r="F85" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I85" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>275</v>
       </c>
@@ -4102,8 +4360,11 @@
       <c r="F86" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I86" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>275</v>
       </c>
@@ -4119,8 +4380,11 @@
       <c r="F87" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I87" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>299</v>
       </c>
@@ -4136,8 +4400,11 @@
       <c r="F88" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I88" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>299</v>
       </c>
@@ -4153,8 +4420,11 @@
       <c r="F89" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I89" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>299</v>
       </c>
@@ -4170,8 +4440,11 @@
       <c r="F90" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I90" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>276</v>
       </c>
@@ -4187,8 +4460,11 @@
       <c r="F91" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I91" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>276</v>
       </c>
@@ -4204,8 +4480,11 @@
       <c r="F92" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I92" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>276</v>
       </c>
@@ -4221,8 +4500,11 @@
       <c r="F93" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I93" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>276</v>
       </c>
@@ -4244,8 +4526,11 @@
       <c r="H94" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I94" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>276</v>
       </c>
@@ -4261,8 +4546,11 @@
       <c r="F95" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I95" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>276</v>
       </c>
@@ -4278,8 +4566,11 @@
       <c r="F96" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I96" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>276</v>
       </c>
@@ -4295,8 +4586,11 @@
       <c r="F97" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I97" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>276</v>
       </c>
@@ -4312,8 +4606,11 @@
       <c r="F98" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I98" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>276</v>
       </c>
@@ -4329,8 +4626,11 @@
       <c r="F99" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I99" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>276</v>
       </c>
@@ -4346,8 +4646,11 @@
       <c r="F100" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I100" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>276</v>
       </c>
@@ -4363,8 +4666,11 @@
       <c r="F101" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I101" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>276</v>
       </c>
@@ -4380,8 +4686,11 @@
       <c r="F102" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I102" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>276</v>
       </c>
@@ -4397,8 +4706,11 @@
       <c r="F103" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I103" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>276</v>
       </c>
@@ -4414,8 +4726,11 @@
       <c r="F104" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I104" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>276</v>
       </c>
@@ -4431,8 +4746,11 @@
       <c r="F105" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I105" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>276</v>
       </c>
@@ -4448,8 +4766,11 @@
       <c r="F106" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I106" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>276</v>
       </c>
@@ -4465,8 +4786,11 @@
       <c r="F107" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I107" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>276</v>
       </c>
@@ -4488,8 +4812,11 @@
       <c r="H108" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I108" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>276</v>
       </c>
@@ -4505,8 +4832,11 @@
       <c r="F109" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I109" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>276</v>
       </c>
@@ -4522,8 +4852,11 @@
       <c r="F110" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I110" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>276</v>
       </c>
@@ -4539,8 +4872,11 @@
       <c r="F111" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I111" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>276</v>
       </c>
@@ -4556,8 +4892,11 @@
       <c r="F112" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I112" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>276</v>
       </c>
@@ -4573,8 +4912,11 @@
       <c r="F113" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I113" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>276</v>
       </c>
@@ -4596,8 +4938,11 @@
       <c r="H114" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I114" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>276</v>
       </c>
@@ -4613,8 +4958,11 @@
       <c r="F115" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I115" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>276</v>
       </c>
@@ -4630,8 +4978,11 @@
       <c r="F116" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I116" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>276</v>
       </c>
@@ -4647,8 +4998,11 @@
       <c r="F117" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I117" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>276</v>
       </c>
@@ -4664,8 +5018,11 @@
       <c r="F118" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I118" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>276</v>
       </c>
@@ -4681,8 +5038,11 @@
       <c r="F119" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I119" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>276</v>
       </c>
@@ -4698,8 +5058,11 @@
       <c r="F120" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I120" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>276</v>
       </c>
@@ -4715,8 +5078,11 @@
       <c r="F121" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I121" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>276</v>
       </c>
@@ -4732,8 +5098,11 @@
       <c r="F122" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I122" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>276</v>
       </c>
@@ -4749,8 +5118,11 @@
       <c r="F123" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I123" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>276</v>
       </c>
@@ -4766,8 +5138,11 @@
       <c r="F124" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I124" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>276</v>
       </c>
@@ -4789,8 +5164,11 @@
       <c r="H125" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I125" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>300</v>
       </c>
@@ -4812,8 +5190,11 @@
       <c r="H126" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I126" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>300</v>
       </c>
@@ -4829,8 +5210,11 @@
       <c r="F127" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I127" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>300</v>
       </c>
@@ -4846,8 +5230,11 @@
       <c r="F128" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I128" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>300</v>
       </c>
@@ -4863,8 +5250,11 @@
       <c r="F129" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I129" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>300</v>
       </c>
@@ -4880,8 +5270,11 @@
       <c r="F130" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I130" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>300</v>
       </c>
@@ -4897,8 +5290,11 @@
       <c r="F131" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I131" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>300</v>
       </c>
@@ -4914,8 +5310,11 @@
       <c r="F132" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I132" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>300</v>
       </c>
@@ -4931,8 +5330,11 @@
       <c r="F133" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I133" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>300</v>
       </c>
@@ -4948,8 +5350,11 @@
       <c r="F134" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I134" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>300</v>
       </c>
@@ -4965,8 +5370,11 @@
       <c r="F135" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I135" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>300</v>
       </c>
@@ -4982,8 +5390,11 @@
       <c r="F136" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I136" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>300</v>
       </c>
@@ -4999,8 +5410,11 @@
       <c r="F137" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I137" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>300</v>
       </c>
@@ -5016,8 +5430,11 @@
       <c r="F138" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I138" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>283</v>
       </c>
@@ -5039,8 +5456,11 @@
       <c r="H139" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I139" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>283</v>
       </c>
@@ -5059,8 +5479,11 @@
       <c r="F140" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I140" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>298</v>
       </c>
@@ -5076,8 +5499,11 @@
       <c r="F141" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I141" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>298</v>
       </c>
@@ -5099,8 +5525,11 @@
       <c r="H142" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I142" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>298</v>
       </c>
@@ -5116,8 +5545,11 @@
       <c r="F143" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I143" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>298</v>
       </c>
@@ -5133,8 +5565,11 @@
       <c r="F144" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I144" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>298</v>
       </c>
@@ -5156,8 +5591,11 @@
       <c r="H145" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I145" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>302</v>
       </c>
@@ -5173,8 +5611,11 @@
       <c r="F146" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I146" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>302</v>
       </c>
@@ -5190,8 +5631,11 @@
       <c r="F147" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I147" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>302</v>
       </c>
@@ -5207,8 +5651,11 @@
       <c r="F148" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I148" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>302</v>
       </c>
@@ -5230,8 +5677,11 @@
       <c r="H149" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I149" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>287</v>
       </c>
@@ -5253,8 +5703,11 @@
       <c r="H150" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I150" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>287</v>
       </c>
@@ -5273,8 +5726,11 @@
       <c r="F151" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I151" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>285</v>
       </c>
@@ -5296,8 +5752,11 @@
       <c r="H152" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I152" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>285</v>
       </c>
@@ -5319,8 +5778,11 @@
       <c r="H153" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I153" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>285</v>
       </c>
@@ -5339,8 +5801,11 @@
       <c r="F154" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I154" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>270</v>
       </c>
@@ -5356,8 +5821,11 @@
       <c r="F155" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I155" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>270</v>
       </c>
@@ -5373,8 +5841,11 @@
       <c r="F156" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I156" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>197</v>
       </c>
@@ -5390,8 +5861,11 @@
       <c r="F157" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I157" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>197</v>
       </c>
@@ -5407,8 +5881,11 @@
       <c r="F158" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I158" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>191</v>
       </c>
@@ -5424,8 +5901,11 @@
       <c r="F159" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I159" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>191</v>
       </c>
@@ -5441,8 +5921,11 @@
       <c r="F160" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I160" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>273</v>
       </c>
@@ -5458,8 +5941,11 @@
       <c r="F161" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I161" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>273</v>
       </c>
@@ -5475,8 +5961,11 @@
       <c r="F162" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I162" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>265</v>
       </c>
@@ -5492,8 +5981,11 @@
       <c r="F163" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I163" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>265</v>
       </c>
@@ -5509,8 +6001,11 @@
       <c r="F164" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I164" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>261</v>
       </c>
@@ -5526,8 +6021,11 @@
       <c r="F165" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I165" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>261</v>
       </c>
@@ -5543,8 +6041,11 @@
       <c r="F166" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I166" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>190</v>
       </c>
@@ -5560,8 +6061,11 @@
       <c r="F167" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I167" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>190</v>
       </c>
@@ -5577,8 +6081,11 @@
       <c r="F168" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I168" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>193</v>
       </c>
@@ -5594,8 +6101,11 @@
       <c r="F169" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I169" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>193</v>
       </c>
@@ -5611,8 +6121,11 @@
       <c r="F170" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I170" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>264</v>
       </c>
@@ -5628,8 +6141,11 @@
       <c r="F171" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I171" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>264</v>
       </c>
@@ -5645,9 +6161,12 @@
       <c r="F172" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="I172" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H172"/>
+  <autoFilter ref="A1:I172"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 'is_scaler' boolean to file specs
</commit_message>
<xml_diff>
--- a/data-raw/flexfile-tables.xlsx
+++ b/data-raw/flexfile-tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="308">
   <si>
     <t>table</t>
   </si>
@@ -944,6 +944,9 @@
   </si>
   <si>
     <t>optional</t>
+  </si>
+  <si>
+    <t>is_scalar</t>
   </si>
 </sst>
 </file>
@@ -1291,11 +1294,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D171"/>
+  <dimension ref="A1:E171"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1306,7 +1307,7 @@
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1319,8 +1320,11 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>291</v>
       </c>
@@ -1333,8 +1337,11 @@
       <c r="D2" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>293</v>
       </c>
@@ -1347,8 +1354,11 @@
       <c r="D3" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>281</v>
       </c>
@@ -1361,8 +1371,11 @@
       <c r="D4" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>280</v>
       </c>
@@ -1375,8 +1388,11 @@
       <c r="D5" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>294</v>
       </c>
@@ -1389,8 +1405,11 @@
       <c r="D6" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>289</v>
       </c>
@@ -1403,8 +1422,11 @@
       <c r="D7" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>295</v>
       </c>
@@ -1417,8 +1439,11 @@
       <c r="D8" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>301</v>
       </c>
@@ -1431,8 +1456,11 @@
       <c r="D9" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>296</v>
       </c>
@@ -1445,8 +1473,11 @@
       <c r="D10" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>297</v>
       </c>
@@ -1459,8 +1490,11 @@
       <c r="D11" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>303</v>
       </c>
@@ -1473,8 +1507,11 @@
       <c r="D12" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>275</v>
       </c>
@@ -1487,8 +1524,11 @@
       <c r="D13" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>299</v>
       </c>
@@ -1501,8 +1541,11 @@
       <c r="D14" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>276</v>
       </c>
@@ -1515,8 +1558,11 @@
       <c r="D15" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>300</v>
       </c>
@@ -1529,8 +1575,11 @@
       <c r="D16" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>283</v>
       </c>
@@ -1543,8 +1592,11 @@
       <c r="D17" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>298</v>
       </c>
@@ -1557,8 +1609,11 @@
       <c r="D18" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>302</v>
       </c>
@@ -1571,8 +1626,11 @@
       <c r="D19" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>287</v>
       </c>
@@ -1585,8 +1643,11 @@
       <c r="D20" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>285</v>
       </c>
@@ -1599,8 +1660,11 @@
       <c r="D21" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>270</v>
       </c>
@@ -1613,8 +1677,11 @@
       <c r="D22" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>197</v>
       </c>
@@ -1627,8 +1694,11 @@
       <c r="D23" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>191</v>
       </c>
@@ -1641,8 +1711,11 @@
       <c r="D24" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>273</v>
       </c>
@@ -1655,8 +1728,11 @@
       <c r="D25" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>265</v>
       </c>
@@ -1669,8 +1745,11 @@
       <c r="D26" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>261</v>
       </c>
@@ -1683,8 +1762,11 @@
       <c r="D27" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>190</v>
       </c>
@@ -1697,8 +1779,11 @@
       <c r="D28" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>193</v>
       </c>
@@ -1711,8 +1796,11 @@
       <c r="D29" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>264</v>
       </c>
@@ -1725,13 +1813,16 @@
       <c r="D30" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="E30" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -2441,9 +2532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5033,7 +5122,7 @@
         <v>101</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="F119" s="4" t="b">
         <v>0</v>
@@ -5133,7 +5222,7 @@
         <v>106</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="F124" s="4" t="b">
         <v>0</v>
@@ -6166,7 +6255,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I172"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added a more generic change_case function
</commit_message>
<xml_diff>
--- a/data-raw/flexfile-tables.xlsx
+++ b/data-raw/flexfile-tables.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DDF657-21B4-4BEA-87C8-8B9C2B346F2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="2" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="402">
   <si>
     <t>table</t>
   </si>
@@ -947,15 +948,310 @@
   </si>
   <si>
     <t>is_scalar</t>
+  </si>
+  <si>
+    <t>excel_3part</t>
+  </si>
+  <si>
+    <t>excel_3part_name</t>
+  </si>
+  <si>
+    <t>Part 1</t>
+  </si>
+  <si>
+    <t>Part 2</t>
+  </si>
+  <si>
+    <t>Part 3</t>
+  </si>
+  <si>
+    <t>Actual Cost-Hour Data</t>
+  </si>
+  <si>
+    <t>Allocation Components</t>
+  </si>
+  <si>
+    <t>Allocation Methods</t>
+  </si>
+  <si>
+    <t>Cost-Hour Tag Definitions</t>
+  </si>
+  <si>
+    <t>End Items</t>
+  </si>
+  <si>
+    <t>FAC Cost-Hour Data</t>
+  </si>
+  <si>
+    <t>Functional Categories</t>
+  </si>
+  <si>
+    <t>Functional Overhead Categories</t>
+  </si>
+  <si>
+    <t>Orders or Lots</t>
+  </si>
+  <si>
+    <t>Report Configuration</t>
+  </si>
+  <si>
+    <t>Reporting Calendar</t>
+  </si>
+  <si>
+    <t>Report Metadata</t>
+  </si>
+  <si>
+    <t>Summary Cost Data</t>
+  </si>
+  <si>
+    <t>Summary Remarks</t>
+  </si>
+  <si>
+    <t>Units or Sublots</t>
+  </si>
+  <si>
+    <t>Work Breakdown Structure</t>
+  </si>
+  <si>
+    <t>WBS Dictionary Definitions</t>
+  </si>
+  <si>
+    <t>WBS Element Remarks</t>
+  </si>
+  <si>
+    <t>Order or Lot ID</t>
+  </si>
+  <si>
+    <t>CLIN ID</t>
+  </si>
+  <si>
+    <t>End Item ID</t>
+  </si>
+  <si>
+    <t>WBS Element ID</t>
+  </si>
+  <si>
+    <t>Account ID</t>
+  </si>
+  <si>
+    <t>Nonrecurring or Recurring ID</t>
+  </si>
+  <si>
+    <t>Functional Category ID</t>
+  </si>
+  <si>
+    <t>Functional
+Overhead Category ID</t>
+  </si>
+  <si>
+    <t>Standard Category ID</t>
+  </si>
+  <si>
+    <t>Detailed
+Standard Category ID</t>
+  </si>
+  <si>
+    <t>Unit or Sublot ID</t>
+  </si>
+  <si>
+    <t>Allocation Method ID</t>
+  </si>
+  <si>
+    <t>Reporting Period ID</t>
+  </si>
+  <si>
+    <t>Tag 1</t>
+  </si>
+  <si>
+    <t>Value (Dollars)</t>
+  </si>
+  <si>
+    <t>Value (Hours)</t>
+  </si>
+  <si>
+    <t>Percent Value</t>
+  </si>
+  <si>
+    <t>Allocation Method
+Type ID</t>
+  </si>
+  <si>
+    <t>Is Unit or Sublot
+Allocation Method</t>
+  </si>
+  <si>
+    <t>Contract Type ID</t>
+  </si>
+  <si>
+    <t>Tag ID</t>
+  </si>
+  <si>
+    <t>Definition Text</t>
+  </si>
+  <si>
+    <t>Phase or Milestone ID</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Contract Price</t>
+  </si>
+  <si>
+    <t>Contract Ceiling</t>
+  </si>
+  <si>
+    <t>Period of Performance
+Start Date</t>
+  </si>
+  <si>
+    <t>Period of Performance
+End Date</t>
+  </si>
+  <si>
+    <t>Appropriation Type ID</t>
+  </si>
+  <si>
+    <t>Detailed Standard Category</t>
+  </si>
+  <si>
+    <t>GA as Standard Category</t>
+  </si>
+  <si>
+    <t>FCCM as Standard Category</t>
+  </si>
+  <si>
+    <t>FAC by Nonrecurring/Recurring</t>
+  </si>
+  <si>
+    <t>FAC by Standard Category</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Security Classification</t>
+  </si>
+  <si>
+    <t>Proprietary Statement</t>
+  </si>
+  <si>
+    <t>Program Name</t>
+  </si>
+  <si>
+    <t>Prime Mission Product</t>
+  </si>
+  <si>
+    <t>Commodity Type</t>
+  </si>
+  <si>
+    <t>Reporting Organization/Organization Name</t>
+  </si>
+  <si>
+    <t>Reporting Organization/Division Name</t>
+  </si>
+  <si>
+    <t>Reporting Organization/CAGE Code</t>
+  </si>
+  <si>
+    <t>Reporting Organization/Location/Street</t>
+  </si>
+  <si>
+    <t>Reporting Organization/Location/City</t>
+  </si>
+  <si>
+    <t>Reporting Organization/Location/State</t>
+  </si>
+  <si>
+    <t>Reporting Organization/Location/Zip Code</t>
+  </si>
+  <si>
+    <t>Reporting Organization/Location/Country</t>
+  </si>
+  <si>
+    <t>Approved Plan Number</t>
+  </si>
+  <si>
+    <t>Approved Plan Revision Number</t>
+  </si>
+  <si>
+    <t>Contract Number</t>
+  </si>
+  <si>
+    <t>Period of Performance/Start Date</t>
+  </si>
+  <si>
+    <t>Period of Performance/End Date</t>
+  </si>
+  <si>
+    <t>Report Cycle ID</t>
+  </si>
+  <si>
+    <t>Submission Event/Number</t>
+  </si>
+  <si>
+    <t>Submission Event/Name</t>
+  </si>
+  <si>
+    <t>Submission Event/Is Wildcard</t>
+  </si>
+  <si>
+    <t>Resubmission Number</t>
+  </si>
+  <si>
+    <t>Report As Of</t>
+  </si>
+  <si>
+    <t>Point of Contact/Name</t>
+  </si>
+  <si>
+    <t>Point of Contact/Department</t>
+  </si>
+  <si>
+    <t>Point of Contact/Telephone Number</t>
+  </si>
+  <si>
+    <t>Point of Contact/Email Address</t>
+  </si>
+  <si>
+    <t>Date Prepared</t>
+  </si>
+  <si>
+    <t>Report Period ID</t>
+  </si>
+  <si>
+    <t>Remarks Text</t>
+  </si>
+  <si>
+    <t>First Unit Number</t>
+  </si>
+  <si>
+    <t>Last Unit Number</t>
+  </si>
+  <si>
+    <t>Parent ID</t>
+  </si>
+  <si>
+    <t>excel_3part_table</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1004,16 +1300,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1293,10 +1593,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E171"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1304,10 +1606,12 @@
     <col min="2" max="2" width="31.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1323,8 +1627,14 @@
       <c r="E1" s="3" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>291</v>
       </c>
@@ -1340,8 +1650,14 @@
       <c r="E2" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>293</v>
       </c>
@@ -1357,8 +1673,14 @@
       <c r="E3" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>281</v>
       </c>
@@ -1374,8 +1696,14 @@
       <c r="E4" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>280</v>
       </c>
@@ -1391,8 +1719,14 @@
       <c r="E5" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>294</v>
       </c>
@@ -1408,8 +1742,14 @@
       <c r="E6" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>289</v>
       </c>
@@ -1425,8 +1765,14 @@
       <c r="E7" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>295</v>
       </c>
@@ -1442,8 +1788,14 @@
       <c r="E8" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>301</v>
       </c>
@@ -1459,8 +1811,14 @@
       <c r="E9" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>296</v>
       </c>
@@ -1476,8 +1834,14 @@
       <c r="E10" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>297</v>
       </c>
@@ -1493,8 +1857,14 @@
       <c r="E11" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>303</v>
       </c>
@@ -1510,8 +1880,14 @@
       <c r="E12" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>275</v>
       </c>
@@ -1527,8 +1903,14 @@
       <c r="E13" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>299</v>
       </c>
@@ -1544,8 +1926,14 @@
       <c r="E14" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>276</v>
       </c>
@@ -1561,8 +1949,14 @@
       <c r="E15" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>300</v>
       </c>
@@ -1578,8 +1972,14 @@
       <c r="E16" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>283</v>
       </c>
@@ -1595,8 +1995,14 @@
       <c r="E17" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>298</v>
       </c>
@@ -1612,8 +2018,14 @@
       <c r="E18" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>302</v>
       </c>
@@ -1629,8 +2041,14 @@
       <c r="E19" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>287</v>
       </c>
@@ -1646,8 +2064,14 @@
       <c r="E20" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>285</v>
       </c>
@@ -1663,8 +2087,14 @@
       <c r="E21" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>270</v>
       </c>
@@ -1681,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>197</v>
       </c>
@@ -1698,7 +2128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>191</v>
       </c>
@@ -1715,7 +2145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>273</v>
       </c>
@@ -1732,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>265</v>
       </c>
@@ -1749,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>261</v>
       </c>
@@ -1766,7 +2196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>190</v>
       </c>
@@ -1783,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>193</v>
       </c>
@@ -1800,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>264</v>
       </c>
@@ -1817,12 +2247,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
     </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -2529,8 +2959,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I172"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2544,10 +2974,12 @@
     <col min="6" max="6" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="9.140625" style="2"/>
+    <col min="10" max="10" width="36" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2575,8 +3007,11 @@
       <c r="I1" s="3" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="9" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>291</v>
       </c>
@@ -2595,8 +3030,11 @@
       <c r="I2" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>291</v>
       </c>
@@ -2615,8 +3053,11 @@
       <c r="I3" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>293</v>
       </c>
@@ -2641,8 +3082,11 @@
       <c r="I4" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>293</v>
       </c>
@@ -2667,8 +3111,11 @@
       <c r="I5" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="10" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>293</v>
       </c>
@@ -2693,8 +3140,11 @@
       <c r="I6" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="10" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>293</v>
       </c>
@@ -2719,8 +3169,11 @@
       <c r="I7" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>293</v>
       </c>
@@ -2745,8 +3198,11 @@
       <c r="I8" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="10" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>293</v>
       </c>
@@ -2771,8 +3227,11 @@
       <c r="I9" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="10" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>293</v>
       </c>
@@ -2797,8 +3256,11 @@
       <c r="I10" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="10" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>293</v>
       </c>
@@ -2823,8 +3285,11 @@
       <c r="I11" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="10" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>293</v>
       </c>
@@ -2849,8 +3314,11 @@
       <c r="I12" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="10" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>293</v>
       </c>
@@ -2875,8 +3343,11 @@
       <c r="I13" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" s="10" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>293</v>
       </c>
@@ -2901,8 +3372,11 @@
       <c r="I14" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" s="10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>293</v>
       </c>
@@ -2927,8 +3401,11 @@
       <c r="I15" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" s="10" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>293</v>
       </c>
@@ -2953,8 +3430,11 @@
       <c r="I16" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="10" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>293</v>
       </c>
@@ -2973,8 +3453,11 @@
       <c r="I17" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="10" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>293</v>
       </c>
@@ -2993,8 +3476,11 @@
       <c r="I18" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="10" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>293</v>
       </c>
@@ -3013,8 +3499,11 @@
       <c r="I19" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>293</v>
       </c>
@@ -3033,8 +3522,11 @@
       <c r="I20" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>293</v>
       </c>
@@ -3053,8 +3545,11 @@
       <c r="I21" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>293</v>
       </c>
@@ -3073,8 +3568,11 @@
       <c r="I22" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>293</v>
       </c>
@@ -3093,8 +3591,11 @@
       <c r="I23" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" s="10" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>293</v>
       </c>
@@ -3113,8 +3614,11 @@
       <c r="I24" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" s="10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>293</v>
       </c>
@@ -3133,8 +3637,11 @@
       <c r="I25" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>293</v>
       </c>
@@ -3153,8 +3660,11 @@
       <c r="I26" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" s="10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>293</v>
       </c>
@@ -3173,8 +3683,11 @@
       <c r="I27" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" s="10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>293</v>
       </c>
@@ -3193,8 +3706,11 @@
       <c r="I28" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" s="10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>293</v>
       </c>
@@ -3213,8 +3729,11 @@
       <c r="I29" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>293</v>
       </c>
@@ -3233,8 +3752,11 @@
       <c r="I30" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" s="10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>293</v>
       </c>
@@ -3253,8 +3775,11 @@
       <c r="I31" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" s="10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>293</v>
       </c>
@@ -3273,8 +3798,11 @@
       <c r="I32" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>293</v>
       </c>
@@ -3293,8 +3821,11 @@
       <c r="I33" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>293</v>
       </c>
@@ -3313,8 +3844,11 @@
       <c r="I34" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" s="10" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>293</v>
       </c>
@@ -3333,8 +3867,11 @@
       <c r="I35" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" s="10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>293</v>
       </c>
@@ -3353,8 +3890,11 @@
       <c r="I36" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>293</v>
       </c>
@@ -3373,8 +3913,11 @@
       <c r="I37" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37" s="10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>293</v>
       </c>
@@ -3393,8 +3936,11 @@
       <c r="I38" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38" s="10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>293</v>
       </c>
@@ -3413,8 +3959,11 @@
       <c r="I39" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>293</v>
       </c>
@@ -3433,8 +3982,11 @@
       <c r="I40" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>293</v>
       </c>
@@ -3453,8 +4005,11 @@
       <c r="I41" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>293</v>
       </c>
@@ -3473,8 +4028,11 @@
       <c r="I42" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42" s="10" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>293</v>
       </c>
@@ -3493,8 +4051,11 @@
       <c r="I43" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43" s="10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>281</v>
       </c>
@@ -3519,8 +4080,11 @@
       <c r="I44" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J44" s="10" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>281</v>
       </c>
@@ -3545,8 +4109,11 @@
       <c r="I45" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45" s="10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>281</v>
       </c>
@@ -3571,8 +4138,11 @@
       <c r="I46" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46" s="10" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>281</v>
       </c>
@@ -3597,8 +4167,11 @@
       <c r="I47" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>281</v>
       </c>
@@ -3623,8 +4196,11 @@
       <c r="I48" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J48" s="10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>281</v>
       </c>
@@ -3643,8 +4219,11 @@
       <c r="I49" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J49" s="10" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>280</v>
       </c>
@@ -3663,8 +4242,11 @@
       <c r="I50" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J50" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>280</v>
       </c>
@@ -3689,8 +4271,11 @@
       <c r="I51" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J51" s="10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>280</v>
       </c>
@@ -3709,8 +4294,11 @@
       <c r="I52" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J52" s="10" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>280</v>
       </c>
@@ -3729,8 +4317,11 @@
       <c r="I53" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J53" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>294</v>
       </c>
@@ -3749,8 +4340,11 @@
       <c r="I54" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J54" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>294</v>
       </c>
@@ -3769,8 +4363,11 @@
       <c r="I55" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J55" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>294</v>
       </c>
@@ -3795,8 +4392,11 @@
       <c r="I56" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J56" s="10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>289</v>
       </c>
@@ -3821,8 +4421,11 @@
       <c r="I57" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J57" s="10" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>289</v>
       </c>
@@ -3841,8 +4444,11 @@
       <c r="I58" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J58" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>289</v>
       </c>
@@ -3864,8 +4470,11 @@
       <c r="I59" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J59" s="10" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>295</v>
       </c>
@@ -3884,8 +4493,11 @@
       <c r="I60" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J60" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>295</v>
       </c>
@@ -3904,8 +4516,11 @@
       <c r="I61" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J61" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>301</v>
       </c>
@@ -3930,8 +4545,11 @@
       <c r="I62" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J62" s="10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>301</v>
       </c>
@@ -3956,8 +4574,11 @@
       <c r="I63" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J63" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>301</v>
       </c>
@@ -3982,8 +4603,11 @@
       <c r="I64" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J64" s="10" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>301</v>
       </c>
@@ -4008,8 +4632,11 @@
       <c r="I65" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J65" s="10" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>301</v>
       </c>
@@ -4034,8 +4661,11 @@
       <c r="I66" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J66" s="10" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>301</v>
       </c>
@@ -4054,8 +4684,11 @@
       <c r="I67" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J67" s="10" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>301</v>
       </c>
@@ -4074,8 +4707,11 @@
       <c r="I68" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J68" s="10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>296</v>
       </c>
@@ -4094,8 +4730,11 @@
       <c r="I69" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J69" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>296</v>
       </c>
@@ -4114,8 +4753,11 @@
       <c r="I70" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J70" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>297</v>
       </c>
@@ -4134,8 +4776,11 @@
       <c r="I71" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J71" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>297</v>
       </c>
@@ -4154,8 +4799,11 @@
       <c r="I72" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J72" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>303</v>
       </c>
@@ -4174,8 +4822,11 @@
       <c r="I73" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J73" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>303</v>
       </c>
@@ -4194,8 +4845,11 @@
       <c r="I74" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J74" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>303</v>
       </c>
@@ -4220,8 +4874,11 @@
       <c r="I75" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J75" s="10" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>303</v>
       </c>
@@ -4240,8 +4897,11 @@
       <c r="I76" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J76" s="10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>303</v>
       </c>
@@ -4266,8 +4926,11 @@
       <c r="I77" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J77" s="10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>303</v>
       </c>
@@ -4286,8 +4949,11 @@
       <c r="I78" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J78" s="10" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>303</v>
       </c>
@@ -4306,8 +4972,11 @@
       <c r="I79" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J79" s="10" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>303</v>
       </c>
@@ -4326,8 +4995,11 @@
       <c r="I80" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J80" s="10" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>303</v>
       </c>
@@ -4346,8 +5018,11 @@
       <c r="I81" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J81" s="10" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>303</v>
       </c>
@@ -4372,8 +5047,11 @@
       <c r="I82" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J82" s="10" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>275</v>
       </c>
@@ -4392,8 +5070,11 @@
       <c r="I83" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J83" s="10" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>275</v>
       </c>
@@ -4412,8 +5093,11 @@
       <c r="I84" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J84" s="10" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>275</v>
       </c>
@@ -4432,8 +5116,11 @@
       <c r="I85" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J85" s="10" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>275</v>
       </c>
@@ -4452,8 +5139,11 @@
       <c r="I86" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J86" s="10" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>275</v>
       </c>
@@ -4472,8 +5162,11 @@
       <c r="I87" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J87" s="10" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>299</v>
       </c>
@@ -4492,8 +5185,11 @@
       <c r="I88" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J88" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>299</v>
       </c>
@@ -4512,8 +5208,11 @@
       <c r="I89" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J89" s="10" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>299</v>
       </c>
@@ -4532,8 +5231,11 @@
       <c r="I90" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J90" s="10" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>276</v>
       </c>
@@ -4552,8 +5254,11 @@
       <c r="I91" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J91" s="10" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>276</v>
       </c>
@@ -4572,8 +5277,11 @@
       <c r="I92" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J92" s="10" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>276</v>
       </c>
@@ -4592,8 +5300,11 @@
       <c r="I93" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J93" s="10" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>276</v>
       </c>
@@ -4618,8 +5329,11 @@
       <c r="I94" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J94" s="10" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>276</v>
       </c>
@@ -4638,8 +5352,11 @@
       <c r="I95" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J95" s="10" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>276</v>
       </c>
@@ -4658,8 +5375,11 @@
       <c r="I96" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J96" s="10" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>276</v>
       </c>
@@ -4678,8 +5398,11 @@
       <c r="I97" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J97" s="10" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>276</v>
       </c>
@@ -4698,8 +5421,11 @@
       <c r="I98" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J98" s="10" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>276</v>
       </c>
@@ -4718,8 +5444,11 @@
       <c r="I99" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J99" s="10" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>276</v>
       </c>
@@ -4738,8 +5467,11 @@
       <c r="I100" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J100" s="10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>276</v>
       </c>
@@ -4758,8 +5490,11 @@
       <c r="I101" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J101" s="10" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>276</v>
       </c>
@@ -4778,8 +5513,11 @@
       <c r="I102" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J102" s="10" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>276</v>
       </c>
@@ -4798,8 +5536,11 @@
       <c r="I103" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J103" s="10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>276</v>
       </c>
@@ -4818,8 +5559,11 @@
       <c r="I104" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J104" s="10" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>276</v>
       </c>
@@ -4838,8 +5582,11 @@
       <c r="I105" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J105" s="10" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>276</v>
       </c>
@@ -4858,8 +5605,11 @@
       <c r="I106" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J106" s="10" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>276</v>
       </c>
@@ -4878,8 +5628,11 @@
       <c r="I107" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J107" s="10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>276</v>
       </c>
@@ -4904,8 +5657,11 @@
       <c r="I108" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J108" s="10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>276</v>
       </c>
@@ -4924,8 +5680,11 @@
       <c r="I109" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J109" s="10" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>276</v>
       </c>
@@ -4944,8 +5703,11 @@
       <c r="I110" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J110" s="10" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>276</v>
       </c>
@@ -4964,8 +5726,11 @@
       <c r="I111" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J111" s="10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>276</v>
       </c>
@@ -4984,8 +5749,11 @@
       <c r="I112" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J112" s="10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>276</v>
       </c>
@@ -5004,8 +5772,11 @@
       <c r="I113" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J113" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>276</v>
       </c>
@@ -5030,8 +5801,11 @@
       <c r="I114" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J114" s="10" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>276</v>
       </c>
@@ -5050,8 +5824,11 @@
       <c r="I115" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J115" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>276</v>
       </c>
@@ -5070,8 +5847,11 @@
       <c r="I116" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J116" s="10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>276</v>
       </c>
@@ -5090,8 +5870,11 @@
       <c r="I117" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J117" s="10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>276</v>
       </c>
@@ -5110,8 +5893,11 @@
       <c r="I118" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J118" s="10" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>276</v>
       </c>
@@ -5130,8 +5916,11 @@
       <c r="I119" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J119" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>276</v>
       </c>
@@ -5150,8 +5939,11 @@
       <c r="I120" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J120" s="10" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>276</v>
       </c>
@@ -5170,8 +5962,11 @@
       <c r="I121" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J121" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>276</v>
       </c>
@@ -5190,8 +5985,11 @@
       <c r="I122" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J122" s="10" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>276</v>
       </c>
@@ -5210,8 +6008,11 @@
       <c r="I123" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J123" s="10" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>276</v>
       </c>
@@ -5230,8 +6031,11 @@
       <c r="I124" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J124" s="10" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>276</v>
       </c>
@@ -5256,8 +6060,11 @@
       <c r="I125" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J125" s="10" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>300</v>
       </c>
@@ -5282,8 +6089,11 @@
       <c r="I126" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J126" s="10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>300</v>
       </c>
@@ -5302,8 +6112,11 @@
       <c r="I127" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J127" s="10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>300</v>
       </c>
@@ -5322,8 +6135,11 @@
       <c r="I128" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J128" s="10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>300</v>
       </c>
@@ -5342,8 +6158,11 @@
       <c r="I129" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J129" s="10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>300</v>
       </c>
@@ -5362,8 +6181,11 @@
       <c r="I130" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J130" s="10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>300</v>
       </c>
@@ -5382,8 +6204,11 @@
       <c r="I131" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J131" s="10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>300</v>
       </c>
@@ -5402,8 +6227,11 @@
       <c r="I132" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J132" s="10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>300</v>
       </c>
@@ -5422,8 +6250,11 @@
       <c r="I133" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J133" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>300</v>
       </c>
@@ -5442,8 +6273,11 @@
       <c r="I134" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J134" s="10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>300</v>
       </c>
@@ -5462,8 +6296,11 @@
       <c r="I135" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J135" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>300</v>
       </c>
@@ -5482,8 +6319,11 @@
       <c r="I136" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J136" s="10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>300</v>
       </c>
@@ -5502,8 +6342,11 @@
       <c r="I137" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J137" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>300</v>
       </c>
@@ -5522,8 +6365,11 @@
       <c r="I138" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J138" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>283</v>
       </c>
@@ -5548,8 +6394,11 @@
       <c r="I139" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J139" s="10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>283</v>
       </c>
@@ -5571,8 +6420,11 @@
       <c r="I140" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J140" s="10" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>298</v>
       </c>
@@ -5591,8 +6443,11 @@
       <c r="I141" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J141" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>298</v>
       </c>
@@ -5617,8 +6472,11 @@
       <c r="I142" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J142" s="10" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>298</v>
       </c>
@@ -5637,8 +6495,11 @@
       <c r="I143" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J143" s="10" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>298</v>
       </c>
@@ -5657,8 +6518,11 @@
       <c r="I144" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J144" s="10" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>298</v>
       </c>
@@ -5683,8 +6547,11 @@
       <c r="I145" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J145" s="10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>302</v>
       </c>
@@ -5703,8 +6570,11 @@
       <c r="I146" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J146" s="10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>302</v>
       </c>
@@ -5723,8 +6593,11 @@
       <c r="I147" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J147" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>302</v>
       </c>
@@ -5743,8 +6616,11 @@
       <c r="I148" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J148" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>302</v>
       </c>
@@ -5769,8 +6645,11 @@
       <c r="I149" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J149" s="10" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>287</v>
       </c>
@@ -5795,8 +6674,11 @@
       <c r="I150" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J150" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>287</v>
       </c>
@@ -5818,8 +6700,11 @@
       <c r="I151" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J151" s="10" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>285</v>
       </c>
@@ -5844,8 +6729,11 @@
       <c r="I152" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J152" s="10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>285</v>
       </c>
@@ -5870,8 +6758,11 @@
       <c r="I153" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J153" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>285</v>
       </c>
@@ -5893,8 +6784,11 @@
       <c r="I154" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J154" s="10" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>270</v>
       </c>
@@ -5913,8 +6807,11 @@
       <c r="I155" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J155" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>270</v>
       </c>
@@ -5933,8 +6830,11 @@
       <c r="I156" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J156" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>197</v>
       </c>
@@ -5953,8 +6853,11 @@
       <c r="I157" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J157" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>197</v>
       </c>
@@ -5973,8 +6876,11 @@
       <c r="I158" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J158" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>191</v>
       </c>
@@ -5993,8 +6899,11 @@
       <c r="I159" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J159" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>191</v>
       </c>
@@ -6013,8 +6922,11 @@
       <c r="I160" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J160" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>273</v>
       </c>
@@ -6033,8 +6945,11 @@
       <c r="I161" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J161" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>273</v>
       </c>
@@ -6053,8 +6968,11 @@
       <c r="I162" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J162" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>265</v>
       </c>
@@ -6073,8 +6991,11 @@
       <c r="I163" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J163" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>265</v>
       </c>
@@ -6093,8 +7014,11 @@
       <c r="I164" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J164" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>261</v>
       </c>
@@ -6113,8 +7037,11 @@
       <c r="I165" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J165" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>261</v>
       </c>
@@ -6133,8 +7060,11 @@
       <c r="I166" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J166" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>190</v>
       </c>
@@ -6153,8 +7083,11 @@
       <c r="I167" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J167" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>190</v>
       </c>
@@ -6173,8 +7106,11 @@
       <c r="I168" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J168" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>193</v>
       </c>
@@ -6193,8 +7129,11 @@
       <c r="I169" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J169" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>193</v>
       </c>
@@ -6213,8 +7152,11 @@
       <c r="I170" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J170" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>264</v>
       </c>
@@ -6233,8 +7175,11 @@
       <c r="I171" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J171" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>264</v>
       </c>
@@ -6252,6 +7197,9 @@
       </c>
       <c r="I172" s="2" t="b">
         <v>0</v>
+      </c>
+      <c r="J172" s="10" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
split enum_spec out of flexfile spec
</commit_message>
<xml_diff>
--- a/data-raw/flexfile-tables.xlsx
+++ b/data-raw/flexfile-tables.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DDF657-21B4-4BEA-87C8-8B9C2B346F2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6202C99A-5E5F-4220-9A15-F416097153AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="fields" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">fields!$A$1:$I$172</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">fields!$A$1:$I$154</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="392">
   <si>
     <t>table</t>
   </si>
@@ -419,33 +419,6 @@
     <t>wbselementremarks</t>
   </si>
   <si>
-    <t>allocationmethodtypeenum</t>
-  </si>
-  <si>
-    <t>appropriationtypeenum</t>
-  </si>
-  <si>
-    <t>contracttypeenum</t>
-  </si>
-  <si>
-    <t>costhourtagenum</t>
-  </si>
-  <si>
-    <t>detailedstandardcategoryenum</t>
-  </si>
-  <si>
-    <t>nonrecurringorrecurringenum</t>
-  </si>
-  <si>
-    <t>phaseormilestoneenum</t>
-  </si>
-  <si>
-    <t>reportcycleenum</t>
-  </si>
-  <si>
-    <t>standardcategoryenum</t>
-  </si>
-  <si>
     <t>safe_name</t>
   </si>
   <si>
@@ -939,9 +912,6 @@
   </si>
   <si>
     <t>submission</t>
-  </si>
-  <si>
-    <t>enum</t>
   </si>
   <si>
     <t>optional</t>
@@ -1594,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G171"/>
+  <dimension ref="A1:G162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1616,636 +1586,528 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>304</v>
-      </c>
-      <c r="E4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F11" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>310</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E13" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E15" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>107</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>120</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>122</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E22" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E23" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E24" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E25" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E26" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E27" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E28" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E29" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E30" s="2" t="b">
-        <v>0</v>
-      </c>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+    </row>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+    </row>
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+    </row>
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A31"/>
@@ -2906,51 +2768,6 @@
       <c r="A162"/>
       <c r="B162"/>
       <c r="C162"/>
-    </row>
-    <row r="163" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A163"/>
-      <c r="B163"/>
-      <c r="C163"/>
-    </row>
-    <row r="164" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A164"/>
-      <c r="B164"/>
-      <c r="C164"/>
-    </row>
-    <row r="165" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A165"/>
-      <c r="B165"/>
-      <c r="C165"/>
-    </row>
-    <row r="166" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A166"/>
-      <c r="B166"/>
-      <c r="C166"/>
-    </row>
-    <row r="167" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A167"/>
-      <c r="B167"/>
-      <c r="C167"/>
-    </row>
-    <row r="168" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A168"/>
-      <c r="B168"/>
-      <c r="C168"/>
-    </row>
-    <row r="169" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A169"/>
-      <c r="B169"/>
-      <c r="C169"/>
-    </row>
-    <row r="170" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A170"/>
-      <c r="B170"/>
-      <c r="C170"/>
-    </row>
-    <row r="171" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A171"/>
-      <c r="B171"/>
-      <c r="C171"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2960,9 +2777,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J172"/>
+  <dimension ref="A1:J154"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2987,10 +2806,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -2999,24 +2818,24 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -3031,15 +2850,15 @@
         <v>0</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -3054,15 +2873,15 @@
         <v>0</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
@@ -3074,24 +2893,24 @@
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
@@ -3103,24 +2922,24 @@
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
@@ -3132,24 +2951,24 @@
         <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>13</v>
@@ -3161,24 +2980,24 @@
         <v>0</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
@@ -3190,24 +3009,24 @@
         <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
@@ -3219,24 +3038,24 @@
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
@@ -3248,24 +3067,24 @@
         <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
@@ -3277,24 +3096,24 @@
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
@@ -3306,24 +3125,24 @@
         <v>0</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
@@ -3335,24 +3154,24 @@
         <v>0</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>20</v>
@@ -3364,24 +3183,24 @@
         <v>0</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
@@ -3393,24 +3212,24 @@
         <v>0</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>22</v>
@@ -3422,24 +3241,24 @@
         <v>0</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>23</v>
@@ -3454,15 +3273,15 @@
         <v>1</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>24</v>
@@ -3477,15 +3296,15 @@
         <v>1</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>25</v>
@@ -3500,15 +3319,15 @@
         <v>1</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>26</v>
@@ -3523,15 +3342,15 @@
         <v>1</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>27</v>
@@ -3546,15 +3365,15 @@
         <v>1</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>28</v>
@@ -3569,15 +3388,15 @@
         <v>1</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>29</v>
@@ -3592,15 +3411,15 @@
         <v>1</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>30</v>
@@ -3615,15 +3434,15 @@
         <v>1</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>31</v>
@@ -3638,15 +3457,15 @@
         <v>1</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>32</v>
@@ -3661,15 +3480,15 @@
         <v>1</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>33</v>
@@ -3684,15 +3503,15 @@
         <v>1</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>34</v>
@@ -3707,15 +3526,15 @@
         <v>1</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>35</v>
@@ -3730,15 +3549,15 @@
         <v>1</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>36</v>
@@ -3753,15 +3572,15 @@
         <v>1</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>37</v>
@@ -3776,15 +3595,15 @@
         <v>1</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>38</v>
@@ -3799,15 +3618,15 @@
         <v>1</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>39</v>
@@ -3822,15 +3641,15 @@
         <v>1</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>40</v>
@@ -3845,15 +3664,15 @@
         <v>1</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>41</v>
@@ -3868,15 +3687,15 @@
         <v>1</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>42</v>
@@ -3891,15 +3710,15 @@
         <v>1</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>43</v>
@@ -3914,15 +3733,15 @@
         <v>1</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>44</v>
@@ -3937,15 +3756,15 @@
         <v>1</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>45</v>
@@ -3960,15 +3779,15 @@
         <v>1</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>46</v>
@@ -3983,15 +3802,15 @@
         <v>1</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>47</v>
@@ -4006,15 +3825,15 @@
         <v>1</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>48</v>
@@ -4029,15 +3848,15 @@
         <v>0</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>50</v>
@@ -4052,15 +3871,15 @@
         <v>0</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>21</v>
@@ -4072,24 +3891,24 @@
         <v>1</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I44" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>10</v>
@@ -4101,24 +3920,24 @@
         <v>1</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I45" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>12</v>
@@ -4130,24 +3949,24 @@
         <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I46" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>13</v>
@@ -4159,24 +3978,24 @@
         <v>1</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I47" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>20</v>
@@ -4188,24 +4007,24 @@
         <v>1</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I48" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>52</v>
@@ -4220,15 +4039,15 @@
         <v>0</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>6</v>
@@ -4243,15 +4062,15 @@
         <v>0</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>54</v>
@@ -4263,24 +4082,24 @@
         <v>0</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I51" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>55</v>
@@ -4295,15 +4114,15 @@
         <v>0</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>8</v>
@@ -4318,15 +4137,15 @@
         <v>0</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>6</v>
@@ -4341,15 +4160,15 @@
         <v>0</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>8</v>
@@ -4364,15 +4183,15 @@
         <v>0</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>58</v>
@@ -4384,24 +4203,24 @@
         <v>0</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I56" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>59</v>
@@ -4413,24 +4232,24 @@
         <v>1</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I57" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>8</v>
@@ -4445,18 +4264,18 @@
         <v>0</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>60</v>
@@ -4471,15 +4290,15 @@
         <v>0</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>6</v>
@@ -4494,15 +4313,15 @@
         <v>0</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>8</v>
@@ -4517,15 +4336,15 @@
         <v>0</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>10</v>
@@ -4537,24 +4356,24 @@
         <v>1</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I62" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>13</v>
@@ -4566,24 +4385,24 @@
         <v>1</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I63" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>15</v>
@@ -4595,24 +4414,24 @@
         <v>1</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I64" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>18</v>
@@ -4624,24 +4443,24 @@
         <v>1</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I65" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>19</v>
@@ -4653,24 +4472,24 @@
         <v>1</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I66" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>48</v>
@@ -4685,15 +4504,15 @@
         <v>0</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>50</v>
@@ -4708,15 +4527,15 @@
         <v>0</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>6</v>
@@ -4731,15 +4550,15 @@
         <v>0</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>8</v>
@@ -4754,15 +4573,15 @@
         <v>0</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>6</v>
@@ -4777,15 +4596,15 @@
         <v>0</v>
       </c>
       <c r="J71" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>8</v>
@@ -4800,15 +4619,15 @@
         <v>0</v>
       </c>
       <c r="J72" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>6</v>
@@ -4823,15 +4642,15 @@
         <v>0</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>8</v>
@@ -4846,15 +4665,15 @@
         <v>0</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>66</v>
@@ -4866,24 +4685,24 @@
         <v>0</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I75" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J75" s="10" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>67</v>
@@ -4898,15 +4717,15 @@
         <v>0</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>58</v>
@@ -4918,24 +4737,24 @@
         <v>0</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I77" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J77" s="10" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>68</v>
@@ -4950,15 +4769,15 @@
         <v>0</v>
       </c>
       <c r="J78" s="10" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>69</v>
@@ -4973,15 +4792,15 @@
         <v>0</v>
       </c>
       <c r="J79" s="10" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>70</v>
@@ -4996,15 +4815,15 @@
         <v>0</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>95</v>
@@ -5019,15 +4838,15 @@
         <v>0</v>
       </c>
       <c r="J81" s="10" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>72</v>
@@ -5039,24 +4858,24 @@
         <v>0</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I82" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>74</v>
@@ -5071,15 +4890,15 @@
         <v>0</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>75</v>
@@ -5094,15 +4913,15 @@
         <v>0</v>
       </c>
       <c r="J84" s="10" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>76</v>
@@ -5117,15 +4936,15 @@
         <v>0</v>
       </c>
       <c r="J85" s="10" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>77</v>
@@ -5140,15 +4959,15 @@
         <v>0</v>
       </c>
       <c r="J86" s="10" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>78</v>
@@ -5163,15 +4982,15 @@
         <v>0</v>
       </c>
       <c r="J87" s="10" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>6</v>
@@ -5186,15 +5005,15 @@
         <v>0</v>
       </c>
       <c r="J88" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>80</v>
@@ -5209,15 +5028,15 @@
         <v>0</v>
       </c>
       <c r="J89" s="10" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>81</v>
@@ -5232,15 +5051,15 @@
         <v>0</v>
       </c>
       <c r="J90" s="10" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>83</v>
@@ -5255,15 +5074,15 @@
         <v>0</v>
       </c>
       <c r="J91" s="10" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>84</v>
@@ -5278,15 +5097,15 @@
         <v>0</v>
       </c>
       <c r="J92" s="10" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>85</v>
@@ -5301,15 +5120,15 @@
         <v>0</v>
       </c>
       <c r="J93" s="10" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>66</v>
@@ -5321,24 +5140,24 @@
         <v>0</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I94" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J94" s="10" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>86</v>
@@ -5353,15 +5172,15 @@
         <v>0</v>
       </c>
       <c r="J95" s="10" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>87</v>
@@ -5376,18 +5195,18 @@
         <v>0</v>
       </c>
       <c r="J96" s="10" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>7</v>
@@ -5399,18 +5218,18 @@
         <v>0</v>
       </c>
       <c r="J97" s="10" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>7</v>
@@ -5422,15 +5241,15 @@
         <v>0</v>
       </c>
       <c r="J98" s="10" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>88</v>
@@ -5445,15 +5264,15 @@
         <v>0</v>
       </c>
       <c r="J99" s="10" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>89</v>
@@ -5468,15 +5287,15 @@
         <v>0</v>
       </c>
       <c r="J100" s="10" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>90</v>
@@ -5491,15 +5310,15 @@
         <v>0</v>
       </c>
       <c r="J101" s="10" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>91</v>
@@ -5514,18 +5333,18 @@
         <v>0</v>
       </c>
       <c r="J102" s="10" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>7</v>
@@ -5537,18 +5356,18 @@
         <v>0</v>
       </c>
       <c r="J103" s="10" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>7</v>
@@ -5560,15 +5379,15 @@
         <v>0</v>
       </c>
       <c r="J104" s="10" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>92</v>
@@ -5583,15 +5402,15 @@
         <v>0</v>
       </c>
       <c r="J105" s="10" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>93</v>
@@ -5606,15 +5425,15 @@
         <v>0</v>
       </c>
       <c r="J106" s="10" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>67</v>
@@ -5629,15 +5448,15 @@
         <v>0</v>
       </c>
       <c r="J107" s="10" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>58</v>
@@ -5649,24 +5468,24 @@
         <v>0</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I108" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J108" s="10" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>68</v>
@@ -5681,15 +5500,15 @@
         <v>0</v>
       </c>
       <c r="J109" s="10" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>69</v>
@@ -5704,15 +5523,15 @@
         <v>0</v>
       </c>
       <c r="J110" s="10" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>94</v>
@@ -5727,15 +5546,15 @@
         <v>0</v>
       </c>
       <c r="J111" s="10" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>70</v>
@@ -5750,15 +5569,15 @@
         <v>0</v>
       </c>
       <c r="J112" s="10" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>95</v>
@@ -5773,15 +5592,15 @@
         <v>0</v>
       </c>
       <c r="J113" s="10" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>96</v>
@@ -5793,24 +5612,24 @@
         <v>0</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I114" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J114" s="10" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>97</v>
@@ -5825,15 +5644,15 @@
         <v>0</v>
       </c>
       <c r="J115" s="10" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>98</v>
@@ -5848,15 +5667,15 @@
         <v>0</v>
       </c>
       <c r="J116" s="10" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>99</v>
@@ -5871,15 +5690,15 @@
         <v>0</v>
       </c>
       <c r="J117" s="10" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>100</v>
@@ -5894,15 +5713,15 @@
         <v>0</v>
       </c>
       <c r="J118" s="10" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>101</v>
@@ -5917,15 +5736,15 @@
         <v>0</v>
       </c>
       <c r="J119" s="10" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>102</v>
@@ -5940,15 +5759,15 @@
         <v>0</v>
       </c>
       <c r="J120" s="10" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>103</v>
@@ -5963,15 +5782,15 @@
         <v>0</v>
       </c>
       <c r="J121" s="10" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>104</v>
@@ -5986,15 +5805,15 @@
         <v>0</v>
       </c>
       <c r="J122" s="10" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>105</v>
@@ -6009,15 +5828,15 @@
         <v>0</v>
       </c>
       <c r="J123" s="10" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>106</v>
@@ -6032,15 +5851,15 @@
         <v>0</v>
       </c>
       <c r="J124" s="10" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>22</v>
@@ -6052,24 +5871,24 @@
         <v>0</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I125" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J125" s="10" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>10</v>
@@ -6081,24 +5900,24 @@
         <v>1</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I126" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J126" s="10" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>108</v>
@@ -6113,15 +5932,15 @@
         <v>0</v>
       </c>
       <c r="J127" s="10" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>109</v>
@@ -6136,15 +5955,15 @@
         <v>0</v>
       </c>
       <c r="J128" s="10" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>110</v>
@@ -6159,15 +5978,15 @@
         <v>0</v>
       </c>
       <c r="J129" s="10" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>111</v>
@@ -6182,15 +6001,15 @@
         <v>0</v>
       </c>
       <c r="J130" s="10" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>112</v>
@@ -6205,15 +6024,15 @@
         <v>0</v>
       </c>
       <c r="J131" s="10" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>113</v>
@@ -6228,15 +6047,15 @@
         <v>0</v>
       </c>
       <c r="J132" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>114</v>
@@ -6251,15 +6070,15 @@
         <v>0</v>
       </c>
       <c r="J133" s="10" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>115</v>
@@ -6274,15 +6093,15 @@
         <v>0</v>
       </c>
       <c r="J134" s="10" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>116</v>
@@ -6297,15 +6116,15 @@
         <v>0</v>
       </c>
       <c r="J135" s="10" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>117</v>
@@ -6320,15 +6139,15 @@
         <v>0</v>
       </c>
       <c r="J136" s="10" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>118</v>
@@ -6343,15 +6162,15 @@
         <v>0</v>
       </c>
       <c r="J137" s="10" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>119</v>
@@ -6366,15 +6185,15 @@
         <v>0</v>
       </c>
       <c r="J138" s="10" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>10</v>
@@ -6386,27 +6205,27 @@
         <v>1</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I139" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J139" s="10" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>121</v>
@@ -6421,15 +6240,15 @@
         <v>0</v>
       </c>
       <c r="J140" s="10" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>6</v>
@@ -6444,15 +6263,15 @@
         <v>0</v>
       </c>
       <c r="J141" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>12</v>
@@ -6464,24 +6283,24 @@
         <v>0</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I142" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J142" s="10" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>123</v>
@@ -6496,15 +6315,15 @@
         <v>0</v>
       </c>
       <c r="J143" s="10" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>124</v>
@@ -6519,15 +6338,15 @@
         <v>0</v>
       </c>
       <c r="J144" s="10" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>10</v>
@@ -6539,24 +6358,24 @@
         <v>0</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="H145" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I145" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J145" s="10" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>126</v>
@@ -6571,15 +6390,15 @@
         <v>0</v>
       </c>
       <c r="J146" s="10" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>6</v>
@@ -6594,15 +6413,15 @@
         <v>0</v>
       </c>
       <c r="J147" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>8</v>
@@ -6617,15 +6436,15 @@
         <v>0</v>
       </c>
       <c r="J148" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>127</v>
@@ -6637,24 +6456,24 @@
         <v>0</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I149" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J149" s="10" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>13</v>
@@ -6666,27 +6485,27 @@
         <v>1</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I150" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J150" s="10" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>129</v>
@@ -6701,15 +6520,15 @@
         <v>0</v>
       </c>
       <c r="J151" s="10" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>10</v>
@@ -6721,24 +6540,24 @@
         <v>1</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I152" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J152" s="10" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>13</v>
@@ -6750,27 +6569,27 @@
         <v>1</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I153" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J153" s="10" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>121</v>
@@ -6785,421 +6604,7 @@
         <v>0</v>
       </c>
       <c r="J154" s="10" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A155" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E155" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F155" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I155" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J155" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A156" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E156" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F156" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I156" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J156" s="10" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A157" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E157" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F157" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I157" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J157" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A158" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E158" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F158" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I158" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J158" s="10" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A159" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E159" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F159" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I159" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J159" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A160" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E160" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F160" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I160" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J160" s="10" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A161" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E161" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F161" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I161" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J161" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A162" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E162" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F162" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I162" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J162" s="10" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A163" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E163" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F163" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I163" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J163" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A164" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E164" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F164" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I164" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J164" s="10" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A165" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E165" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F165" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I165" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J165" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A166" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F166" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I166" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J166" s="10" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A167" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E167" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F167" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I167" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J167" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A168" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E168" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F168" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I168" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J168" s="10" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A169" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E169" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F169" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I169" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J169" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A170" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E170" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F170" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I170" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J170" s="10" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A171" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E171" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F171" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I171" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J171" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A172" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C172" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E172" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F172" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I172" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J172" s="10" t="s">
-        <v>195</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Better way to filter checks
</commit_message>
<xml_diff>
--- a/data-raw/flexfile-tables.xlsx
+++ b/data-raw/flexfile-tables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6202C99A-5E5F-4220-9A15-F416097153AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D143D55-E52C-4F7A-85F5-CE534B7446CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="402">
   <si>
     <t>table</t>
   </si>
@@ -1206,15 +1206,52 @@
   </si>
   <si>
     <t>excel_3part_table</t>
+  </si>
+  <si>
+    <t>allocationmethodtypeenum</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>appropriationtypeenum</t>
+  </si>
+  <si>
+    <t>contracttypeenum</t>
+  </si>
+  <si>
+    <t>costhourtagenum</t>
+  </si>
+  <si>
+    <t>detailedstandardcategoryenum</t>
+  </si>
+  <si>
+    <t>nonrecurringorrecurringenum</t>
+  </si>
+  <si>
+    <t>phaseormilestoneenum</t>
+  </si>
+  <si>
+    <t>reportcycleenum</t>
+  </si>
+  <si>
+    <t>standardcategoryenum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1272,17 +1309,17 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1564,25 +1601,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G162"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="24.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="9"/>
+    <col min="7" max="7" width="26.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1591,1183 +1626,631 @@
       <c r="C1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="E3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="9" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="E6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="9" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="9" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="9" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="9" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E10" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="9" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="9" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E12" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7" t="s">
+      <c r="E12" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="9" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E13" s="2" t="b">
+      <c r="E13" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="9" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="7" t="s">
+      <c r="E14" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="9" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E15" s="2" t="b">
+      <c r="E15" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="9" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E16" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7" t="s">
+      <c r="E16" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="9" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E17" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7" t="s">
+      <c r="E17" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="9" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="7" t="s">
+      <c r="E18" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="9" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7" t="s">
+      <c r="E19" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="9" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E20" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7" t="s">
+      <c r="E20" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="9" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7" t="s">
+      <c r="E21" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="9" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-    </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-    </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-    </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-    </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-    </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-    </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-    </row>
-    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-    </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-    </row>
-    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-    </row>
-    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-    </row>
-    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-    </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-    </row>
-    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-    </row>
-    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-    </row>
-    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-    </row>
-    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-    </row>
-    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42"/>
-      <c r="B42"/>
-      <c r="C42"/>
-    </row>
-    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43"/>
-      <c r="B43"/>
-      <c r="C43"/>
-    </row>
-    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
-    </row>
-    <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45"/>
-      <c r="B45"/>
-      <c r="C45"/>
-    </row>
-    <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46"/>
-      <c r="B46"/>
-      <c r="C46"/>
-    </row>
-    <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
-    </row>
-    <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48"/>
-      <c r="B48"/>
-      <c r="C48"/>
-    </row>
-    <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49"/>
-      <c r="B49"/>
-      <c r="C49"/>
-    </row>
-    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50"/>
-      <c r="B50"/>
-      <c r="C50"/>
-    </row>
-    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51"/>
-      <c r="B51"/>
-      <c r="C51"/>
-    </row>
-    <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52"/>
-      <c r="B52"/>
-      <c r="C52"/>
-    </row>
-    <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53"/>
-      <c r="B53"/>
-      <c r="C53"/>
-    </row>
-    <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54"/>
-      <c r="B54"/>
-      <c r="C54"/>
-    </row>
-    <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55"/>
-      <c r="B55"/>
-      <c r="C55"/>
-    </row>
-    <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56"/>
-    </row>
-    <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57"/>
-      <c r="B57"/>
-      <c r="C57"/>
-    </row>
-    <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58"/>
-      <c r="B58"/>
-      <c r="C58"/>
-    </row>
-    <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59"/>
-      <c r="B59"/>
-      <c r="C59"/>
-    </row>
-    <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
-    </row>
-    <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
-    </row>
-    <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62"/>
-      <c r="B62"/>
-      <c r="C62"/>
-    </row>
-    <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63"/>
-      <c r="B63"/>
-      <c r="C63"/>
-    </row>
-    <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64"/>
-      <c r="B64"/>
-      <c r="C64"/>
-    </row>
-    <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65"/>
-      <c r="B65"/>
-      <c r="C65"/>
-    </row>
-    <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66"/>
-      <c r="B66"/>
-      <c r="C66"/>
-    </row>
-    <row r="67" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67"/>
-      <c r="B67"/>
-      <c r="C67"/>
-    </row>
-    <row r="68" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68"/>
-      <c r="B68"/>
-      <c r="C68"/>
-    </row>
-    <row r="69" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69"/>
-      <c r="B69"/>
-      <c r="C69"/>
-    </row>
-    <row r="70" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70"/>
-      <c r="B70"/>
-      <c r="C70"/>
-    </row>
-    <row r="71" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71"/>
-      <c r="B71"/>
-      <c r="C71"/>
-    </row>
-    <row r="72" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72"/>
-      <c r="B72"/>
-      <c r="C72"/>
-    </row>
-    <row r="73" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73"/>
-      <c r="B73"/>
-      <c r="C73"/>
-    </row>
-    <row r="74" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74"/>
-      <c r="B74"/>
-      <c r="C74"/>
-    </row>
-    <row r="75" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75"/>
-      <c r="B75"/>
-      <c r="C75"/>
-    </row>
-    <row r="76" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76"/>
-      <c r="B76"/>
-      <c r="C76"/>
-    </row>
-    <row r="77" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77"/>
-      <c r="B77"/>
-      <c r="C77"/>
-    </row>
-    <row r="78" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78"/>
-      <c r="B78"/>
-      <c r="C78"/>
-    </row>
-    <row r="79" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79"/>
-      <c r="B79"/>
-      <c r="C79"/>
-    </row>
-    <row r="80" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80"/>
-      <c r="B80"/>
-      <c r="C80"/>
-    </row>
-    <row r="81" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81"/>
-      <c r="B81"/>
-      <c r="C81"/>
-    </row>
-    <row r="82" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82"/>
-      <c r="B82"/>
-      <c r="C82"/>
-    </row>
-    <row r="83" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83"/>
-      <c r="B83"/>
-      <c r="C83"/>
-    </row>
-    <row r="84" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84"/>
-      <c r="B84"/>
-      <c r="C84"/>
-    </row>
-    <row r="85" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85"/>
-      <c r="B85"/>
-      <c r="C85"/>
-    </row>
-    <row r="86" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86"/>
-      <c r="B86"/>
-      <c r="C86"/>
-    </row>
-    <row r="87" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87"/>
-      <c r="B87"/>
-      <c r="C87"/>
-    </row>
-    <row r="88" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="C88"/>
-    </row>
-    <row r="89" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89"/>
-      <c r="B89"/>
-      <c r="C89"/>
-    </row>
-    <row r="90" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90"/>
-      <c r="B90"/>
-      <c r="C90"/>
-    </row>
-    <row r="91" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91"/>
-      <c r="B91"/>
-      <c r="C91"/>
-    </row>
-    <row r="92" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92"/>
-      <c r="B92"/>
-      <c r="C92"/>
-    </row>
-    <row r="93" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93"/>
-      <c r="B93"/>
-      <c r="C93"/>
-    </row>
-    <row r="94" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94"/>
-      <c r="B94"/>
-      <c r="C94"/>
-    </row>
-    <row r="95" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95"/>
-      <c r="B95"/>
-      <c r="C95"/>
-    </row>
-    <row r="96" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96"/>
-      <c r="B96"/>
-      <c r="C96"/>
-    </row>
-    <row r="97" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97"/>
-      <c r="B97"/>
-      <c r="C97"/>
-    </row>
-    <row r="98" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98"/>
-      <c r="B98"/>
-      <c r="C98"/>
-    </row>
-    <row r="99" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99"/>
-      <c r="B99"/>
-      <c r="C99"/>
-    </row>
-    <row r="100" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100"/>
-      <c r="B100"/>
-      <c r="C100"/>
-    </row>
-    <row r="101" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101"/>
-      <c r="B101"/>
-      <c r="C101"/>
-    </row>
-    <row r="102" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102"/>
-      <c r="B102"/>
-      <c r="C102"/>
-    </row>
-    <row r="103" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A103"/>
-      <c r="B103"/>
-      <c r="C103"/>
-    </row>
-    <row r="104" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104"/>
-      <c r="B104"/>
-      <c r="C104"/>
-    </row>
-    <row r="105" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105"/>
-      <c r="B105"/>
-      <c r="C105"/>
-    </row>
-    <row r="106" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106"/>
-      <c r="B106"/>
-      <c r="C106"/>
-    </row>
-    <row r="107" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107"/>
-      <c r="B107"/>
-      <c r="C107"/>
-    </row>
-    <row r="108" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108"/>
-      <c r="B108"/>
-      <c r="C108"/>
-    </row>
-    <row r="109" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109"/>
-      <c r="B109"/>
-      <c r="C109"/>
-    </row>
-    <row r="110" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110"/>
-      <c r="B110"/>
-      <c r="C110"/>
-    </row>
-    <row r="111" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111"/>
-      <c r="B111"/>
-      <c r="C111"/>
-    </row>
-    <row r="112" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112"/>
-      <c r="B112"/>
-      <c r="C112"/>
-    </row>
-    <row r="113" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113"/>
-      <c r="B113"/>
-      <c r="C113"/>
-    </row>
-    <row r="114" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114"/>
-      <c r="B114"/>
-      <c r="C114"/>
-    </row>
-    <row r="115" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115"/>
-      <c r="B115"/>
-      <c r="C115"/>
-    </row>
-    <row r="116" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A116"/>
-      <c r="B116"/>
-      <c r="C116"/>
-    </row>
-    <row r="117" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A117"/>
-      <c r="B117"/>
-      <c r="C117"/>
-    </row>
-    <row r="118" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A118"/>
-      <c r="B118"/>
-      <c r="C118"/>
-    </row>
-    <row r="119" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A119"/>
-      <c r="B119"/>
-      <c r="C119"/>
-    </row>
-    <row r="120" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A120"/>
-      <c r="B120"/>
-      <c r="C120"/>
-    </row>
-    <row r="121" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A121"/>
-      <c r="B121"/>
-      <c r="C121"/>
-    </row>
-    <row r="122" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A122"/>
-      <c r="B122"/>
-      <c r="C122"/>
-    </row>
-    <row r="123" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A123"/>
-      <c r="B123"/>
-      <c r="C123"/>
-    </row>
-    <row r="124" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A124"/>
-      <c r="B124"/>
-      <c r="C124"/>
-    </row>
-    <row r="125" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A125"/>
-      <c r="B125"/>
-      <c r="C125"/>
-    </row>
-    <row r="126" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A126"/>
-      <c r="B126"/>
-      <c r="C126"/>
-    </row>
-    <row r="127" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A127"/>
-      <c r="B127"/>
-      <c r="C127"/>
-    </row>
-    <row r="128" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A128"/>
-      <c r="B128"/>
-      <c r="C128"/>
-    </row>
-    <row r="129" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A129"/>
-      <c r="B129"/>
-      <c r="C129"/>
-    </row>
-    <row r="130" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A130"/>
-      <c r="B130"/>
-      <c r="C130"/>
-    </row>
-    <row r="131" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A131"/>
-      <c r="B131"/>
-      <c r="C131"/>
-    </row>
-    <row r="132" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A132"/>
-      <c r="B132"/>
-      <c r="C132"/>
-    </row>
-    <row r="133" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A133"/>
-      <c r="B133"/>
-      <c r="C133"/>
-    </row>
-    <row r="134" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A134"/>
-      <c r="B134"/>
-      <c r="C134"/>
-    </row>
-    <row r="135" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A135"/>
-      <c r="B135"/>
-      <c r="C135"/>
-    </row>
-    <row r="136" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A136"/>
-      <c r="B136"/>
-      <c r="C136"/>
-    </row>
-    <row r="137" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A137"/>
-      <c r="B137"/>
-      <c r="C137"/>
-    </row>
-    <row r="138" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A138"/>
-      <c r="B138"/>
-      <c r="C138"/>
-    </row>
-    <row r="139" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A139"/>
-      <c r="B139"/>
-      <c r="C139"/>
-    </row>
-    <row r="140" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A140"/>
-      <c r="B140"/>
-      <c r="C140"/>
-    </row>
-    <row r="141" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A141"/>
-      <c r="B141"/>
-      <c r="C141"/>
-    </row>
-    <row r="142" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A142"/>
-      <c r="B142"/>
-      <c r="C142"/>
-    </row>
-    <row r="143" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A143"/>
-      <c r="B143"/>
-      <c r="C143"/>
-    </row>
-    <row r="144" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A144"/>
-      <c r="B144"/>
-      <c r="C144"/>
-    </row>
-    <row r="145" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A145"/>
-      <c r="B145"/>
-      <c r="C145"/>
-    </row>
-    <row r="146" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A146"/>
-      <c r="B146"/>
-      <c r="C146"/>
-    </row>
-    <row r="147" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A147"/>
-      <c r="B147"/>
-      <c r="C147"/>
-    </row>
-    <row r="148" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A148"/>
-      <c r="B148"/>
-      <c r="C148"/>
-    </row>
-    <row r="149" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A149"/>
-      <c r="B149"/>
-      <c r="C149"/>
-    </row>
-    <row r="150" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A150"/>
-      <c r="B150"/>
-      <c r="C150"/>
-    </row>
-    <row r="151" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A151"/>
-      <c r="B151"/>
-      <c r="C151"/>
-    </row>
-    <row r="152" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A152"/>
-      <c r="B152"/>
-      <c r="C152"/>
-    </row>
-    <row r="153" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A153"/>
-      <c r="B153"/>
-      <c r="C153"/>
-    </row>
-    <row r="154" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A154"/>
-      <c r="B154"/>
-      <c r="C154"/>
-    </row>
-    <row r="155" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A155"/>
-      <c r="B155"/>
-      <c r="C155"/>
-    </row>
-    <row r="156" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A156"/>
-      <c r="B156"/>
-      <c r="C156"/>
-    </row>
-    <row r="157" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A157"/>
-      <c r="B157"/>
-      <c r="C157"/>
-    </row>
-    <row r="158" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A158"/>
-      <c r="B158"/>
-      <c r="C158"/>
-    </row>
-    <row r="159" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A159"/>
-      <c r="B159"/>
-      <c r="C159"/>
-    </row>
-    <row r="160" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A160"/>
-      <c r="B160"/>
-      <c r="C160"/>
-    </row>
-    <row r="161" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A161"/>
-      <c r="B161"/>
-      <c r="C161"/>
-    </row>
-    <row r="162" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A162"/>
-      <c r="B162"/>
-      <c r="C162"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="E22" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="E23" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="E24" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="E25" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="E26" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="E27" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="E28" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="E29" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="E30" s="9" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2777,11 +2260,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J154"/>
+  <dimension ref="A1:J172"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2826,7 +2307,7 @@
       <c r="I1" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>299</v>
       </c>
     </row>
@@ -2849,7 +2330,7 @@
       <c r="I2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="8" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2872,7 +2353,7 @@
       <c r="I3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="8" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2901,7 +2382,7 @@
       <c r="I4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="8" t="s">
         <v>321</v>
       </c>
     </row>
@@ -2930,7 +2411,7 @@
       <c r="I5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="8" t="s">
         <v>322</v>
       </c>
     </row>
@@ -2959,7 +2440,7 @@
       <c r="I6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="8" t="s">
         <v>323</v>
       </c>
     </row>
@@ -2988,7 +2469,7 @@
       <c r="I7" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="8" t="s">
         <v>324</v>
       </c>
     </row>
@@ -3017,7 +2498,7 @@
       <c r="I8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="8" t="s">
         <v>325</v>
       </c>
     </row>
@@ -3046,7 +2527,7 @@
       <c r="I9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="8" t="s">
         <v>326</v>
       </c>
     </row>
@@ -3075,7 +2556,7 @@
       <c r="I10" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="8" t="s">
         <v>327</v>
       </c>
     </row>
@@ -3104,7 +2585,7 @@
       <c r="I11" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="8" t="s">
         <v>328</v>
       </c>
     </row>
@@ -3133,7 +2614,7 @@
       <c r="I12" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="8" t="s">
         <v>329</v>
       </c>
     </row>
@@ -3162,7 +2643,7 @@
       <c r="I13" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="8" t="s">
         <v>330</v>
       </c>
     </row>
@@ -3191,7 +2672,7 @@
       <c r="I14" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="8" t="s">
         <v>331</v>
       </c>
     </row>
@@ -3220,7 +2701,7 @@
       <c r="I15" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="8" t="s">
         <v>332</v>
       </c>
     </row>
@@ -3249,7 +2730,7 @@
       <c r="I16" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="8" t="s">
         <v>333</v>
       </c>
     </row>
@@ -3272,7 +2753,7 @@
       <c r="I17" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="8" t="s">
         <v>334</v>
       </c>
     </row>
@@ -3295,7 +2776,7 @@
       <c r="I18" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="8" t="s">
         <v>214</v>
       </c>
     </row>
@@ -3318,7 +2799,7 @@
       <c r="I19" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="8" t="s">
         <v>215</v>
       </c>
     </row>
@@ -3341,7 +2822,7 @@
       <c r="I20" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="8" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3364,7 +2845,7 @@
       <c r="I21" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="J21" s="8" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3387,7 +2868,7 @@
       <c r="I22" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="8" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3410,7 +2891,7 @@
       <c r="I23" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J23" s="10" t="s">
+      <c r="J23" s="8" t="s">
         <v>219</v>
       </c>
     </row>
@@ -3433,7 +2914,7 @@
       <c r="I24" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="J24" s="8" t="s">
         <v>220</v>
       </c>
     </row>
@@ -3456,7 +2937,7 @@
       <c r="I25" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="8" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3479,7 +2960,7 @@
       <c r="I26" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="J26" s="8" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3502,7 +2983,7 @@
       <c r="I27" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J27" s="10" t="s">
+      <c r="J27" s="8" t="s">
         <v>223</v>
       </c>
     </row>
@@ -3525,7 +3006,7 @@
       <c r="I28" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J28" s="10" t="s">
+      <c r="J28" s="8" t="s">
         <v>224</v>
       </c>
     </row>
@@ -3548,7 +3029,7 @@
       <c r="I29" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J29" s="10" t="s">
+      <c r="J29" s="8" t="s">
         <v>225</v>
       </c>
     </row>
@@ -3571,7 +3052,7 @@
       <c r="I30" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J30" s="10" t="s">
+      <c r="J30" s="8" t="s">
         <v>226</v>
       </c>
     </row>
@@ -3594,7 +3075,7 @@
       <c r="I31" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J31" s="10" t="s">
+      <c r="J31" s="8" t="s">
         <v>227</v>
       </c>
     </row>
@@ -3617,7 +3098,7 @@
       <c r="I32" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="J32" s="8" t="s">
         <v>228</v>
       </c>
     </row>
@@ -3640,7 +3121,7 @@
       <c r="I33" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J33" s="10" t="s">
+      <c r="J33" s="8" t="s">
         <v>229</v>
       </c>
     </row>
@@ -3663,7 +3144,7 @@
       <c r="I34" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J34" s="10" t="s">
+      <c r="J34" s="8" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3686,7 +3167,7 @@
       <c r="I35" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J35" s="10" t="s">
+      <c r="J35" s="8" t="s">
         <v>231</v>
       </c>
     </row>
@@ -3709,7 +3190,7 @@
       <c r="I36" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J36" s="10" t="s">
+      <c r="J36" s="8" t="s">
         <v>232</v>
       </c>
     </row>
@@ -3732,7 +3213,7 @@
       <c r="I37" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J37" s="10" t="s">
+      <c r="J37" s="8" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3755,7 +3236,7 @@
       <c r="I38" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J38" s="10" t="s">
+      <c r="J38" s="8" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3778,7 +3259,7 @@
       <c r="I39" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J39" s="10" t="s">
+      <c r="J39" s="8" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3801,7 +3282,7 @@
       <c r="I40" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J40" s="10" t="s">
+      <c r="J40" s="8" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3824,7 +3305,7 @@
       <c r="I41" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J41" s="10" t="s">
+      <c r="J41" s="8" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3847,7 +3328,7 @@
       <c r="I42" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J42" s="10" t="s">
+      <c r="J42" s="8" t="s">
         <v>335</v>
       </c>
     </row>
@@ -3870,7 +3351,7 @@
       <c r="I43" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J43" s="10" t="s">
+      <c r="J43" s="8" t="s">
         <v>336</v>
       </c>
     </row>
@@ -3899,7 +3380,7 @@
       <c r="I44" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J44" s="10" t="s">
+      <c r="J44" s="8" t="s">
         <v>332</v>
       </c>
     </row>
@@ -3928,7 +3409,7 @@
       <c r="I45" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J45" s="10" t="s">
+      <c r="J45" s="8" t="s">
         <v>321</v>
       </c>
     </row>
@@ -3957,7 +3438,7 @@
       <c r="I46" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J46" s="10" t="s">
+      <c r="J46" s="8" t="s">
         <v>323</v>
       </c>
     </row>
@@ -3986,7 +3467,7 @@
       <c r="I47" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J47" s="10" t="s">
+      <c r="J47" s="8" t="s">
         <v>324</v>
       </c>
     </row>
@@ -4015,7 +3496,7 @@
       <c r="I48" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J48" s="10" t="s">
+      <c r="J48" s="8" t="s">
         <v>331</v>
       </c>
     </row>
@@ -4038,7 +3519,7 @@
       <c r="I49" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J49" s="10" t="s">
+      <c r="J49" s="8" t="s">
         <v>337</v>
       </c>
     </row>
@@ -4061,7 +3542,7 @@
       <c r="I50" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J50" s="10" t="s">
+      <c r="J50" s="8" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4090,7 +3571,7 @@
       <c r="I51" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J51" s="10" t="s">
+      <c r="J51" s="8" t="s">
         <v>338</v>
       </c>
     </row>
@@ -4113,7 +3594,7 @@
       <c r="I52" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J52" s="10" t="s">
+      <c r="J52" s="8" t="s">
         <v>339</v>
       </c>
     </row>
@@ -4136,7 +3617,7 @@
       <c r="I53" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J53" s="10" t="s">
+      <c r="J53" s="8" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4159,7 +3640,7 @@
       <c r="I54" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J54" s="10" t="s">
+      <c r="J54" s="8" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4182,7 +3663,7 @@
       <c r="I55" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J55" s="10" t="s">
+      <c r="J55" s="8" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4211,7 +3692,7 @@
       <c r="I56" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J56" s="10" t="s">
+      <c r="J56" s="8" t="s">
         <v>340</v>
       </c>
     </row>
@@ -4240,7 +3721,7 @@
       <c r="I57" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J57" s="10" t="s">
+      <c r="J57" s="8" t="s">
         <v>341</v>
       </c>
     </row>
@@ -4263,7 +3744,7 @@
       <c r="I58" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J58" s="10" t="s">
+      <c r="J58" s="8" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4289,7 +3770,7 @@
       <c r="I59" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J59" s="10" t="s">
+      <c r="J59" s="8" t="s">
         <v>342</v>
       </c>
     </row>
@@ -4312,7 +3793,7 @@
       <c r="I60" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J60" s="10" t="s">
+      <c r="J60" s="8" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4335,7 +3816,7 @@
       <c r="I61" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J61" s="10" t="s">
+      <c r="J61" s="8" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4364,7 +3845,7 @@
       <c r="I62" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J62" s="10" t="s">
+      <c r="J62" s="8" t="s">
         <v>321</v>
       </c>
     </row>
@@ -4393,7 +3874,7 @@
       <c r="I63" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J63" s="10" t="s">
+      <c r="J63" s="8" t="s">
         <v>324</v>
       </c>
     </row>
@@ -4422,7 +3903,7 @@
       <c r="I64" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J64" s="10" t="s">
+      <c r="J64" s="8" t="s">
         <v>326</v>
       </c>
     </row>
@@ -4451,7 +3932,7 @@
       <c r="I65" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J65" s="10" t="s">
+      <c r="J65" s="8" t="s">
         <v>329</v>
       </c>
     </row>
@@ -4480,7 +3961,7 @@
       <c r="I66" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J66" s="10" t="s">
+      <c r="J66" s="8" t="s">
         <v>330</v>
       </c>
     </row>
@@ -4503,7 +3984,7 @@
       <c r="I67" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J67" s="10" t="s">
+      <c r="J67" s="8" t="s">
         <v>335</v>
       </c>
     </row>
@@ -4526,7 +4007,7 @@
       <c r="I68" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J68" s="10" t="s">
+      <c r="J68" s="8" t="s">
         <v>336</v>
       </c>
     </row>
@@ -4549,7 +4030,7 @@
       <c r="I69" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J69" s="10" t="s">
+      <c r="J69" s="8" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4572,7 +4053,7 @@
       <c r="I70" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J70" s="10" t="s">
+      <c r="J70" s="8" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4595,7 +4076,7 @@
       <c r="I71" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J71" s="10" t="s">
+      <c r="J71" s="8" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4618,7 +4099,7 @@
       <c r="I72" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J72" s="10" t="s">
+      <c r="J72" s="8" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4641,7 +4122,7 @@
       <c r="I73" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J73" s="10" t="s">
+      <c r="J73" s="8" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4664,7 +4145,7 @@
       <c r="I74" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J74" s="10" t="s">
+      <c r="J74" s="8" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4693,7 +4174,7 @@
       <c r="I75" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J75" s="10" t="s">
+      <c r="J75" s="8" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4716,7 +4197,7 @@
       <c r="I76" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J76" s="10" t="s">
+      <c r="J76" s="8" t="s">
         <v>344</v>
       </c>
     </row>
@@ -4745,7 +4226,7 @@
       <c r="I77" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J77" s="10" t="s">
+      <c r="J77" s="8" t="s">
         <v>340</v>
       </c>
     </row>
@@ -4768,7 +4249,7 @@
       <c r="I78" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J78" s="10" t="s">
+      <c r="J78" s="8" t="s">
         <v>345</v>
       </c>
     </row>
@@ -4791,7 +4272,7 @@
       <c r="I79" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J79" s="10" t="s">
+      <c r="J79" s="8" t="s">
         <v>346</v>
       </c>
     </row>
@@ -4814,7 +4295,7 @@
       <c r="I80" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J80" s="10" t="s">
+      <c r="J80" s="8" t="s">
         <v>347</v>
       </c>
     </row>
@@ -4837,7 +4318,7 @@
       <c r="I81" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J81" s="10" t="s">
+      <c r="J81" s="8" t="s">
         <v>348</v>
       </c>
     </row>
@@ -4866,7 +4347,7 @@
       <c r="I82" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J82" s="10" t="s">
+      <c r="J82" s="8" t="s">
         <v>349</v>
       </c>
     </row>
@@ -4889,7 +4370,7 @@
       <c r="I83" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J83" s="10" t="s">
+      <c r="J83" s="8" t="s">
         <v>350</v>
       </c>
     </row>
@@ -4912,7 +4393,7 @@
       <c r="I84" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J84" s="10" t="s">
+      <c r="J84" s="8" t="s">
         <v>351</v>
       </c>
     </row>
@@ -4935,7 +4416,7 @@
       <c r="I85" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J85" s="10" t="s">
+      <c r="J85" s="8" t="s">
         <v>352</v>
       </c>
     </row>
@@ -4958,7 +4439,7 @@
       <c r="I86" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J86" s="10" t="s">
+      <c r="J86" s="8" t="s">
         <v>353</v>
       </c>
     </row>
@@ -4981,7 +4462,7 @@
       <c r="I87" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J87" s="10" t="s">
+      <c r="J87" s="8" t="s">
         <v>354</v>
       </c>
     </row>
@@ -5004,7 +4485,7 @@
       <c r="I88" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J88" s="10" t="s">
+      <c r="J88" s="8" t="s">
         <v>183</v>
       </c>
     </row>
@@ -5027,7 +4508,7 @@
       <c r="I89" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J89" s="10" t="s">
+      <c r="J89" s="8" t="s">
         <v>355</v>
       </c>
     </row>
@@ -5050,7 +4531,7 @@
       <c r="I90" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J90" s="10" t="s">
+      <c r="J90" s="8" t="s">
         <v>356</v>
       </c>
     </row>
@@ -5073,7 +4554,7 @@
       <c r="I91" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J91" s="10" t="s">
+      <c r="J91" s="8" t="s">
         <v>357</v>
       </c>
     </row>
@@ -5096,7 +4577,7 @@
       <c r="I92" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J92" s="10" t="s">
+      <c r="J92" s="8" t="s">
         <v>358</v>
       </c>
     </row>
@@ -5119,7 +4600,7 @@
       <c r="I93" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J93" s="10" t="s">
+      <c r="J93" s="8" t="s">
         <v>359</v>
       </c>
     </row>
@@ -5148,7 +4629,7 @@
       <c r="I94" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J94" s="10" t="s">
+      <c r="J94" s="8" t="s">
         <v>343</v>
       </c>
     </row>
@@ -5171,7 +4652,7 @@
       <c r="I95" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J95" s="10" t="s">
+      <c r="J95" s="8" t="s">
         <v>360</v>
       </c>
     </row>
@@ -5194,7 +4675,7 @@
       <c r="I96" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J96" s="10" t="s">
+      <c r="J96" s="8" t="s">
         <v>361</v>
       </c>
     </row>
@@ -5217,7 +4698,7 @@
       <c r="I97" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J97" s="10" t="s">
+      <c r="J97" s="8" t="s">
         <v>362</v>
       </c>
     </row>
@@ -5240,7 +4721,7 @@
       <c r="I98" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J98" s="10" t="s">
+      <c r="J98" s="8" t="s">
         <v>363</v>
       </c>
     </row>
@@ -5263,7 +4744,7 @@
       <c r="I99" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J99" s="10" t="s">
+      <c r="J99" s="8" t="s">
         <v>364</v>
       </c>
     </row>
@@ -5286,7 +4767,7 @@
       <c r="I100" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J100" s="10" t="s">
+      <c r="J100" s="8" t="s">
         <v>365</v>
       </c>
     </row>
@@ -5309,7 +4790,7 @@
       <c r="I101" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J101" s="10" t="s">
+      <c r="J101" s="8" t="s">
         <v>366</v>
       </c>
     </row>
@@ -5332,7 +4813,7 @@
       <c r="I102" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J102" s="10" t="s">
+      <c r="J102" s="8" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5355,7 +4836,7 @@
       <c r="I103" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J103" s="10" t="s">
+      <c r="J103" s="8" t="s">
         <v>368</v>
       </c>
     </row>
@@ -5378,7 +4859,7 @@
       <c r="I104" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J104" s="10" t="s">
+      <c r="J104" s="8" t="s">
         <v>369</v>
       </c>
     </row>
@@ -5401,7 +4882,7 @@
       <c r="I105" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J105" s="10" t="s">
+      <c r="J105" s="8" t="s">
         <v>370</v>
       </c>
     </row>
@@ -5424,7 +4905,7 @@
       <c r="I106" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J106" s="10" t="s">
+      <c r="J106" s="8" t="s">
         <v>371</v>
       </c>
     </row>
@@ -5447,7 +4928,7 @@
       <c r="I107" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J107" s="10" t="s">
+      <c r="J107" s="8" t="s">
         <v>344</v>
       </c>
     </row>
@@ -5476,7 +4957,7 @@
       <c r="I108" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J108" s="10" t="s">
+      <c r="J108" s="8" t="s">
         <v>340</v>
       </c>
     </row>
@@ -5499,7 +4980,7 @@
       <c r="I109" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J109" s="10" t="s">
+      <c r="J109" s="8" t="s">
         <v>345</v>
       </c>
     </row>
@@ -5522,7 +5003,7 @@
       <c r="I110" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J110" s="10" t="s">
+      <c r="J110" s="8" t="s">
         <v>346</v>
       </c>
     </row>
@@ -5545,7 +5026,7 @@
       <c r="I111" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J111" s="10" t="s">
+      <c r="J111" s="8" t="s">
         <v>372</v>
       </c>
     </row>
@@ -5568,7 +5049,7 @@
       <c r="I112" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J112" s="10" t="s">
+      <c r="J112" s="8" t="s">
         <v>373</v>
       </c>
     </row>
@@ -5591,7 +5072,7 @@
       <c r="I113" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J113" s="10" t="s">
+      <c r="J113" s="8" t="s">
         <v>374</v>
       </c>
     </row>
@@ -5620,7 +5101,7 @@
       <c r="I114" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J114" s="10" t="s">
+      <c r="J114" s="8" t="s">
         <v>375</v>
       </c>
     </row>
@@ -5643,7 +5124,7 @@
       <c r="I115" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J115" s="10" t="s">
+      <c r="J115" s="8" t="s">
         <v>376</v>
       </c>
     </row>
@@ -5666,7 +5147,7 @@
       <c r="I116" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J116" s="10" t="s">
+      <c r="J116" s="8" t="s">
         <v>377</v>
       </c>
     </row>
@@ -5689,7 +5170,7 @@
       <c r="I117" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J117" s="10" t="s">
+      <c r="J117" s="8" t="s">
         <v>378</v>
       </c>
     </row>
@@ -5712,7 +5193,7 @@
       <c r="I118" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J118" s="10" t="s">
+      <c r="J118" s="8" t="s">
         <v>379</v>
       </c>
     </row>
@@ -5735,7 +5216,7 @@
       <c r="I119" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J119" s="10" t="s">
+      <c r="J119" s="8" t="s">
         <v>380</v>
       </c>
     </row>
@@ -5758,7 +5239,7 @@
       <c r="I120" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J120" s="10" t="s">
+      <c r="J120" s="8" t="s">
         <v>381</v>
       </c>
     </row>
@@ -5781,7 +5262,7 @@
       <c r="I121" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J121" s="10" t="s">
+      <c r="J121" s="8" t="s">
         <v>382</v>
       </c>
     </row>
@@ -5804,7 +5285,7 @@
       <c r="I122" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J122" s="10" t="s">
+      <c r="J122" s="8" t="s">
         <v>383</v>
       </c>
     </row>
@@ -5827,7 +5308,7 @@
       <c r="I123" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J123" s="10" t="s">
+      <c r="J123" s="8" t="s">
         <v>384</v>
       </c>
     </row>
@@ -5850,7 +5331,7 @@
       <c r="I124" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J124" s="10" t="s">
+      <c r="J124" s="8" t="s">
         <v>385</v>
       </c>
     </row>
@@ -5879,7 +5360,7 @@
       <c r="I125" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J125" s="10" t="s">
+      <c r="J125" s="8" t="s">
         <v>386</v>
       </c>
     </row>
@@ -5908,7 +5389,7 @@
       <c r="I126" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J126" s="10" t="s">
+      <c r="J126" s="8" t="s">
         <v>321</v>
       </c>
     </row>
@@ -5931,7 +5412,7 @@
       <c r="I127" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J127" s="10" t="s">
+      <c r="J127" s="8" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5954,7 +5435,7 @@
       <c r="I128" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J128" s="10" t="s">
+      <c r="J128" s="8" t="s">
         <v>202</v>
       </c>
     </row>
@@ -5977,7 +5458,7 @@
       <c r="I129" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J129" s="10" t="s">
+      <c r="J129" s="8" t="s">
         <v>203</v>
       </c>
     </row>
@@ -6000,7 +5481,7 @@
       <c r="I130" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J130" s="10" t="s">
+      <c r="J130" s="8" t="s">
         <v>204</v>
       </c>
     </row>
@@ -6023,7 +5504,7 @@
       <c r="I131" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J131" s="10" t="s">
+      <c r="J131" s="8" t="s">
         <v>205</v>
       </c>
     </row>
@@ -6046,7 +5527,7 @@
       <c r="I132" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J132" s="10" t="s">
+      <c r="J132" s="8" t="s">
         <v>206</v>
       </c>
     </row>
@@ -6069,7 +5550,7 @@
       <c r="I133" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J133" s="10" t="s">
+      <c r="J133" s="8" t="s">
         <v>207</v>
       </c>
     </row>
@@ -6092,7 +5573,7 @@
       <c r="I134" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J134" s="10" t="s">
+      <c r="J134" s="8" t="s">
         <v>208</v>
       </c>
     </row>
@@ -6115,7 +5596,7 @@
       <c r="I135" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J135" s="10" t="s">
+      <c r="J135" s="8" t="s">
         <v>209</v>
       </c>
     </row>
@@ -6138,7 +5619,7 @@
       <c r="I136" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J136" s="10" t="s">
+      <c r="J136" s="8" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6161,7 +5642,7 @@
       <c r="I137" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J137" s="10" t="s">
+      <c r="J137" s="8" t="s">
         <v>211</v>
       </c>
     </row>
@@ -6184,7 +5665,7 @@
       <c r="I138" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J138" s="10" t="s">
+      <c r="J138" s="8" t="s">
         <v>212</v>
       </c>
     </row>
@@ -6213,7 +5694,7 @@
       <c r="I139" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J139" s="10" t="s">
+      <c r="J139" s="8" t="s">
         <v>321</v>
       </c>
     </row>
@@ -6239,7 +5720,7 @@
       <c r="I140" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J140" s="10" t="s">
+      <c r="J140" s="8" t="s">
         <v>387</v>
       </c>
     </row>
@@ -6262,7 +5743,7 @@
       <c r="I141" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J141" s="10" t="s">
+      <c r="J141" s="8" t="s">
         <v>183</v>
       </c>
     </row>
@@ -6291,7 +5772,7 @@
       <c r="I142" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J142" s="10" t="s">
+      <c r="J142" s="8" t="s">
         <v>323</v>
       </c>
     </row>
@@ -6314,7 +5795,7 @@
       <c r="I143" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J143" s="10" t="s">
+      <c r="J143" s="8" t="s">
         <v>388</v>
       </c>
     </row>
@@ -6337,7 +5818,7 @@
       <c r="I144" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J144" s="10" t="s">
+      <c r="J144" s="8" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6366,7 +5847,7 @@
       <c r="I145" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J145" s="10" t="s">
+      <c r="J145" s="8" t="s">
         <v>321</v>
       </c>
     </row>
@@ -6389,7 +5870,7 @@
       <c r="I146" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J146" s="10" t="s">
+      <c r="J146" s="8" t="s">
         <v>189</v>
       </c>
     </row>
@@ -6412,7 +5893,7 @@
       <c r="I147" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J147" s="10" t="s">
+      <c r="J147" s="8" t="s">
         <v>183</v>
       </c>
     </row>
@@ -6435,7 +5916,7 @@
       <c r="I148" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J148" s="10" t="s">
+      <c r="J148" s="8" t="s">
         <v>186</v>
       </c>
     </row>
@@ -6464,7 +5945,7 @@
       <c r="I149" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J149" s="10" t="s">
+      <c r="J149" s="8" t="s">
         <v>390</v>
       </c>
     </row>
@@ -6493,7 +5974,7 @@
       <c r="I150" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J150" s="10" t="s">
+      <c r="J150" s="8" t="s">
         <v>324</v>
       </c>
     </row>
@@ -6519,7 +6000,7 @@
       <c r="I151" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J151" s="10" t="s">
+      <c r="J151" s="8" t="s">
         <v>342</v>
       </c>
     </row>
@@ -6548,7 +6029,7 @@
       <c r="I152" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J152" s="10" t="s">
+      <c r="J152" s="8" t="s">
         <v>321</v>
       </c>
     </row>
@@ -6577,7 +6058,7 @@
       <c r="I153" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J153" s="10" t="s">
+      <c r="J153" s="8" t="s">
         <v>324</v>
       </c>
     </row>
@@ -6603,8 +6084,422 @@
       <c r="I154" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J154" s="10" t="s">
+      <c r="J154" s="8" t="s">
         <v>387</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A155" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C155" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D155" s="9"/>
+      <c r="E155" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F155" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G155" s="9"/>
+      <c r="H155" s="9"/>
+      <c r="I155" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A156" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="B156" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D156" s="9"/>
+      <c r="E156" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F156" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G156" s="9"/>
+      <c r="H156" s="9"/>
+      <c r="I156" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A157" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B157" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D157" s="9"/>
+      <c r="E157" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F157" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G157" s="9"/>
+      <c r="H157" s="9"/>
+      <c r="I157" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A158" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D158" s="9"/>
+      <c r="E158" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F158" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G158" s="9"/>
+      <c r="H158" s="9"/>
+      <c r="I158" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A159" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C159" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D159" s="9"/>
+      <c r="E159" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F159" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G159" s="9"/>
+      <c r="H159" s="9"/>
+      <c r="I159" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A160" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C160" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D160" s="9"/>
+      <c r="E160" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F160" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G160" s="9"/>
+      <c r="H160" s="9"/>
+      <c r="I160" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A161" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C161" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D161" s="9"/>
+      <c r="E161" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F161" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G161" s="9"/>
+      <c r="H161" s="9"/>
+      <c r="I161" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A162" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C162" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D162" s="9"/>
+      <c r="E162" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F162" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G162" s="9"/>
+      <c r="H162" s="9"/>
+      <c r="I162" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A163" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="B163" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C163" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D163" s="9"/>
+      <c r="E163" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F163" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G163" s="9"/>
+      <c r="H163" s="9"/>
+      <c r="I163" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A164" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="B164" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C164" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D164" s="9"/>
+      <c r="E164" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F164" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G164" s="9"/>
+      <c r="H164" s="9"/>
+      <c r="I164" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A165" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B165" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C165" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D165" s="9"/>
+      <c r="E165" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F165" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G165" s="9"/>
+      <c r="H165" s="9"/>
+      <c r="I165" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A166" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B166" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C166" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D166" s="9"/>
+      <c r="E166" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F166" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G166" s="9"/>
+      <c r="H166" s="9"/>
+      <c r="I166" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A167" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B167" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C167" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D167" s="9"/>
+      <c r="E167" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F167" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G167" s="9"/>
+      <c r="H167" s="9"/>
+      <c r="I167" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A168" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B168" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C168" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D168" s="9"/>
+      <c r="E168" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F168" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G168" s="9"/>
+      <c r="H168" s="9"/>
+      <c r="I168" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A169" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B169" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C169" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D169" s="9"/>
+      <c r="E169" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F169" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G169" s="9"/>
+      <c r="H169" s="9"/>
+      <c r="I169" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A170" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B170" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C170" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D170" s="9"/>
+      <c r="E170" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F170" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G170" s="9"/>
+      <c r="H170" s="9"/>
+      <c r="I170" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A171" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B171" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C171" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D171" s="9"/>
+      <c r="E171" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F171" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G171" s="9"/>
+      <c r="H171" s="9"/>
+      <c r="I171" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A172" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B172" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C172" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D172" s="9"/>
+      <c r="E172" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F172" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G172" s="9"/>
+      <c r="H172" s="9"/>
+      <c r="I172" s="9" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>